<commit_message>
Update TitanX pascal numbers with GEMM fix and new CUDA/driver version.
</commit_message>
<xml_diff>
--- a/results/DeepBench_NV_TitanX_Pascal.xlsx
+++ b/results/DeepBench_NV_TitanX_Pascal.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="14940" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="63">
   <si>
     <t>Dense Matrix Multiplication</t>
   </si>
@@ -280,8 +280,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="249">
+  <cellStyleXfs count="285">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -549,7 +585,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="249">
+  <cellStyles count="285">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -674,6 +710,24 @@
     <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -798,6 +852,24 @@
     <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1127,11 +1199,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC172"/>
+  <dimension ref="A1:AE172"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="AA90" sqref="AA90:AD126"/>
-    </sheetView>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1150,7 +1220,7 @@
     <col min="22" max="22" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1176,7 +1246,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:12">
       <c r="C2">
         <v>1760</v>
       </c>
@@ -1199,8 +1269,10 @@
         <f>(2*C2*D2*E2)/(I2/1000)/10^12</f>
         <v>1.982464</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="C3">
         <v>1760</v>
       </c>
@@ -1217,14 +1289,16 @@
         <v>3</v>
       </c>
       <c r="I3" s="2">
-        <v>0.113</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="J3" s="2">
         <f t="shared" ref="J3:J66" si="0">(2*C3*D3*E3)/(I3/1000)/10^12</f>
-        <v>1.7543929203539821</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>0.97658325123152712</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="C4">
         <v>1760</v>
       </c>
@@ -1241,14 +1315,16 @@
         <v>3</v>
       </c>
       <c r="I4" s="2">
-        <v>0.16300000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="J4" s="2">
         <f t="shared" si="0"/>
-        <v>2.4324711656441718</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>3.964928</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="C5">
         <v>1760</v>
       </c>
@@ -1265,14 +1341,16 @@
         <v>3</v>
       </c>
       <c r="I5" s="2">
-        <v>0.17</v>
+        <v>0.107</v>
       </c>
       <c r="J5" s="2">
         <f t="shared" si="0"/>
-        <v>4.6646211764705878</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>7.4110803738317754</v>
+      </c>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="C6">
         <v>1760</v>
       </c>
@@ -1289,14 +1367,16 @@
         <v>3</v>
       </c>
       <c r="I6" s="2">
-        <v>4.4740000000000002</v>
+        <v>4.2990000000000004</v>
       </c>
       <c r="J6" s="2">
         <f t="shared" si="0"/>
-        <v>9.6929816718819843</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10">
+        <v>10.087555245405905</v>
+      </c>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="C7">
         <v>2048</v>
       </c>
@@ -1313,14 +1393,16 @@
         <v>3</v>
       </c>
       <c r="I7" s="2">
-        <v>9.4E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="J7" s="2">
         <f t="shared" si="0"/>
-        <v>1.4278481702127661</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
+        <v>1.4749200879120878</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="C8">
         <v>2048</v>
       </c>
@@ -1337,14 +1419,16 @@
         <v>3</v>
       </c>
       <c r="I8" s="2">
-        <v>0.113</v>
+        <v>0.20899999999999999</v>
       </c>
       <c r="J8" s="2">
         <f t="shared" si="0"/>
-        <v>2.3755350088495573</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
+        <v>1.284380172248804</v>
+      </c>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="C9">
         <v>2048</v>
       </c>
@@ -1361,14 +1445,16 @@
         <v>3</v>
       </c>
       <c r="I9" s="2">
-        <v>0.222</v>
+        <v>0.182</v>
       </c>
       <c r="J9" s="2">
         <f t="shared" si="0"/>
-        <v>2.4183374414414414</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
+        <v>2.9498401758241757</v>
+      </c>
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+    </row>
+    <row r="10" spans="1:12">
       <c r="C10">
         <v>2048</v>
       </c>
@@ -1385,14 +1471,16 @@
         <v>3</v>
       </c>
       <c r="I10" s="2">
-        <v>0.182</v>
+        <v>0.14899999999999999</v>
       </c>
       <c r="J10" s="2">
         <f t="shared" si="0"/>
-        <v>5.8996803516483514</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+        <v>7.2063209664429531</v>
+      </c>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="C11">
         <v>2048</v>
       </c>
@@ -1409,14 +1497,16 @@
         <v>3</v>
       </c>
       <c r="I11" s="2">
-        <v>5.44</v>
+        <v>5.5309999999999997</v>
       </c>
       <c r="J11" s="2">
         <f t="shared" si="0"/>
-        <v>10.794164705882352</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
+        <v>10.61657132525764</v>
+      </c>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="C12">
         <v>2560</v>
       </c>
@@ -1433,14 +1523,16 @@
         <v>3</v>
       </c>
       <c r="I12" s="2">
-        <v>0.16300000000000001</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="J12" s="2">
         <f t="shared" si="0"/>
-        <v>1.2865963190184049</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
+        <v>1.2945382716049383</v>
+      </c>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+    </row>
+    <row r="13" spans="1:12">
       <c r="C13">
         <v>2560</v>
       </c>
@@ -1457,14 +1549,16 @@
         <v>3</v>
       </c>
       <c r="I13" s="2">
-        <v>0.17199999999999999</v>
+        <v>0.26400000000000001</v>
       </c>
       <c r="J13" s="2">
         <f t="shared" si="0"/>
-        <v>2.4385488372093027</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>1.588751515151515</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
+    </row>
+    <row r="14" spans="1:12">
       <c r="C14">
         <v>2560</v>
       </c>
@@ -1481,14 +1575,16 @@
         <v>3</v>
       </c>
       <c r="I14" s="2">
-        <v>0.27800000000000002</v>
+        <v>0.29799999999999999</v>
       </c>
       <c r="J14" s="2">
         <f t="shared" si="0"/>
-        <v>3.0174848920863306</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+        <v>2.814969127516779</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="C15">
         <v>2560</v>
       </c>
@@ -1505,14 +1601,16 @@
         <v>3</v>
       </c>
       <c r="I15" s="2">
-        <v>0.23799999999999999</v>
+        <v>0.29599999999999999</v>
       </c>
       <c r="J15" s="2">
         <f t="shared" si="0"/>
-        <v>7.0492504201680672</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>5.667978378378379</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="C16">
         <v>2560</v>
       </c>
@@ -1529,14 +1627,16 @@
         <v>3</v>
       </c>
       <c r="I16" s="2">
-        <v>9.2940000000000005</v>
+        <v>8.9879999999999995</v>
       </c>
       <c r="J16" s="2">
         <f t="shared" si="0"/>
-        <v>9.8720034430815584</v>
-      </c>
-    </row>
-    <row r="17" spans="3:10">
+        <v>10.208099688473521</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+    </row>
+    <row r="17" spans="3:12">
       <c r="C17">
         <v>4096</v>
       </c>
@@ -1553,14 +1653,16 @@
         <v>3</v>
       </c>
       <c r="I17" s="2">
-        <v>0.48899999999999999</v>
+        <v>0.48799999999999999</v>
       </c>
       <c r="J17" s="2">
         <f t="shared" si="0"/>
-        <v>1.0978955255623724</v>
-      </c>
-    </row>
-    <row r="18" spans="3:10">
+        <v>1.1001453114754098</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+    </row>
+    <row r="18" spans="3:12">
       <c r="C18">
         <v>4096</v>
       </c>
@@ -1577,14 +1679,16 @@
         <v>3</v>
       </c>
       <c r="I18" s="2">
-        <v>0.40500000000000003</v>
+        <v>0.495</v>
       </c>
       <c r="J18" s="2">
         <f t="shared" si="0"/>
-        <v>2.6512143802469135</v>
-      </c>
-    </row>
-    <row r="19" spans="3:10">
+        <v>2.1691754020202021</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+    </row>
+    <row r="19" spans="3:12">
       <c r="C19">
         <v>4096</v>
       </c>
@@ -1601,14 +1705,16 @@
         <v>3</v>
       </c>
       <c r="I19" s="2">
-        <v>0.442</v>
+        <v>0.496</v>
       </c>
       <c r="J19" s="2">
         <f t="shared" si="0"/>
-        <v>4.8585602895927602</v>
-      </c>
-    </row>
-    <row r="20" spans="3:10">
+        <v>4.3296041290322576</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+    </row>
+    <row r="20" spans="3:12">
       <c r="C20">
         <v>4096</v>
       </c>
@@ -1625,14 +1731,16 @@
         <v>3</v>
       </c>
       <c r="I20" s="2">
-        <v>0.53400000000000003</v>
+        <v>0.65200000000000002</v>
       </c>
       <c r="J20" s="2">
         <f t="shared" si="0"/>
-        <v>8.0430099176029959</v>
-      </c>
-    </row>
-    <row r="21" spans="3:10">
+        <v>6.5873731533742337</v>
+      </c>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+    </row>
+    <row r="21" spans="3:12">
       <c r="C21">
         <v>4096</v>
       </c>
@@ -1649,14 +1757,16 @@
         <v>3</v>
       </c>
       <c r="I21" s="2">
-        <v>24.116</v>
+        <v>22.95</v>
       </c>
       <c r="J21" s="2">
         <f t="shared" si="0"/>
-        <v>9.7396344335710747</v>
-      </c>
-    </row>
-    <row r="22" spans="3:10">
+        <v>10.234467276688454</v>
+      </c>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+    </row>
+    <row r="22" spans="3:12">
       <c r="C22">
         <v>1760</v>
       </c>
@@ -1673,14 +1783,16 @@
         <v>3</v>
       </c>
       <c r="I22" s="2">
-        <v>0.14799999999999999</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="J22" s="2">
         <f t="shared" si="0"/>
-        <v>0.66975135135135144</v>
-      </c>
-    </row>
-    <row r="23" spans="3:10">
+        <v>1.0218886597938144</v>
+      </c>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+    </row>
+    <row r="23" spans="3:12">
       <c r="C23">
         <v>1760</v>
       </c>
@@ -1697,14 +1809,16 @@
         <v>3</v>
       </c>
       <c r="I23" s="2">
-        <v>0.122</v>
+        <v>0.156</v>
       </c>
       <c r="J23" s="2">
         <f t="shared" si="0"/>
-        <v>1.6249704918032788</v>
-      </c>
-    </row>
-    <row r="24" spans="3:10">
+        <v>1.2708102564102564</v>
+      </c>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+    </row>
+    <row r="24" spans="3:12">
       <c r="C24">
         <v>1760</v>
       </c>
@@ -1721,14 +1835,16 @@
         <v>3</v>
       </c>
       <c r="I24" s="2">
-        <v>0.14399999999999999</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="J24" s="2">
         <f t="shared" si="0"/>
-        <v>2.7534222222222224</v>
-      </c>
-    </row>
-    <row r="25" spans="3:10">
+        <v>1.9435921568627452</v>
+      </c>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+    </row>
+    <row r="25" spans="3:12">
       <c r="C25">
         <v>1760</v>
       </c>
@@ -1745,14 +1861,16 @@
         <v>3</v>
       </c>
       <c r="I25" s="2">
-        <v>0.27400000000000002</v>
+        <v>0.22900000000000001</v>
       </c>
       <c r="J25" s="2">
         <f t="shared" si="0"/>
-        <v>2.8941080291970795</v>
-      </c>
-    </row>
-    <row r="26" spans="3:10">
+        <v>3.4628192139737988</v>
+      </c>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+    </row>
+    <row r="26" spans="3:12">
       <c r="C26">
         <v>1760</v>
       </c>
@@ -1769,14 +1887,16 @@
         <v>3</v>
       </c>
       <c r="I26" s="2">
-        <v>4.8890000000000002</v>
+        <v>4.7439999999999998</v>
       </c>
       <c r="J26" s="2">
         <f t="shared" si="0"/>
-        <v>8.8701984045817124</v>
-      </c>
-    </row>
-    <row r="27" spans="3:10">
+        <v>9.141315345699832</v>
+      </c>
+      <c r="K26" s="2"/>
+      <c r="L26" s="2"/>
+    </row>
+    <row r="27" spans="3:12">
       <c r="C27">
         <v>2048</v>
       </c>
@@ -1793,14 +1913,16 @@
         <v>3</v>
       </c>
       <c r="I27" s="2">
-        <v>0.14099999999999999</v>
+        <v>0.112</v>
       </c>
       <c r="J27" s="2">
         <f t="shared" si="0"/>
-        <v>0.95189878014184415</v>
-      </c>
-    </row>
-    <row r="28" spans="3:10">
+        <v>1.1983725714285716</v>
+      </c>
+      <c r="K27" s="2"/>
+      <c r="L27" s="2"/>
+    </row>
+    <row r="28" spans="3:12">
       <c r="C28">
         <v>2048</v>
       </c>
@@ -1817,14 +1939,16 @@
         <v>3</v>
       </c>
       <c r="I28" s="2">
-        <v>9.7000000000000003E-2</v>
+        <v>0.22600000000000001</v>
       </c>
       <c r="J28" s="2">
         <f t="shared" si="0"/>
-        <v>2.7673758350515465</v>
-      </c>
-    </row>
-    <row r="29" spans="3:10">
+        <v>1.1877675044247786</v>
+      </c>
+      <c r="K28" s="2"/>
+      <c r="L28" s="2"/>
+    </row>
+    <row r="29" spans="3:12">
       <c r="C29">
         <v>2048</v>
       </c>
@@ -1841,14 +1965,16 @@
         <v>3</v>
       </c>
       <c r="I29" s="2">
-        <v>0.216</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="J29" s="2">
         <f t="shared" si="0"/>
-        <v>2.4855134814814814</v>
-      </c>
-    </row>
-    <row r="30" spans="3:10">
+        <v>1.5606712558139537</v>
+      </c>
+      <c r="K29" s="2"/>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="3:12">
       <c r="C30">
         <v>2048</v>
       </c>
@@ -1865,14 +1991,16 @@
         <v>3</v>
       </c>
       <c r="I30" s="2">
-        <v>0.25</v>
+        <v>0.20399999999999999</v>
       </c>
       <c r="J30" s="2">
         <f t="shared" si="0"/>
-        <v>4.2949672960000003</v>
-      </c>
-    </row>
-    <row r="31" spans="3:10">
+        <v>5.2634403137254901</v>
+      </c>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+    </row>
+    <row r="31" spans="3:12">
       <c r="C31">
         <v>2048</v>
       </c>
@@ -1889,14 +2017,16 @@
         <v>3</v>
       </c>
       <c r="I31" s="2">
-        <v>6.0720000000000001</v>
+        <v>5.77</v>
       </c>
       <c r="J31" s="2">
         <f t="shared" si="0"/>
-        <v>9.6706613965744399</v>
-      </c>
-    </row>
-    <row r="32" spans="3:10">
+        <v>10.176820797227037</v>
+      </c>
+      <c r="K31" s="2"/>
+      <c r="L31" s="2"/>
+    </row>
+    <row r="32" spans="3:12">
       <c r="C32">
         <v>2560</v>
       </c>
@@ -1913,14 +2043,16 @@
         <v>3</v>
       </c>
       <c r="I32" s="2">
-        <v>0.29399999999999998</v>
+        <v>0.183</v>
       </c>
       <c r="J32" s="2">
         <f t="shared" si="0"/>
-        <v>0.71331700680272103</v>
-      </c>
-    </row>
-    <row r="33" spans="3:10">
+        <v>1.1459846994535521</v>
+      </c>
+      <c r="K32" s="2"/>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="3:12">
       <c r="C33">
         <v>2560</v>
       </c>
@@ -1937,14 +2069,16 @@
         <v>3</v>
       </c>
       <c r="I33" s="2">
-        <v>0.23899999999999999</v>
+        <v>0.3</v>
       </c>
       <c r="J33" s="2">
         <f t="shared" si="0"/>
-        <v>1.7549389121338914</v>
-      </c>
-    </row>
-    <row r="34" spans="3:10">
+        <v>1.3981013333333334</v>
+      </c>
+      <c r="K33" s="2"/>
+      <c r="L33" s="2"/>
+    </row>
+    <row r="34" spans="3:12">
       <c r="C34">
         <v>2560</v>
       </c>
@@ -1961,14 +2095,16 @@
         <v>3</v>
       </c>
       <c r="I34" s="2">
-        <v>0.33900000000000002</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="J34" s="2">
         <f t="shared" si="0"/>
-        <v>2.4745156342182892</v>
-      </c>
-    </row>
-    <row r="35" spans="3:10">
+        <v>2.8926234482758617</v>
+      </c>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+    </row>
+    <row r="35" spans="3:12">
       <c r="C35">
         <v>2560</v>
       </c>
@@ -1985,14 +2121,16 @@
         <v>3</v>
       </c>
       <c r="I35" s="2">
-        <v>0.57299999999999995</v>
+        <v>0.53100000000000003</v>
       </c>
       <c r="J35" s="2">
         <f t="shared" si="0"/>
-        <v>2.9279609075043633</v>
-      </c>
-    </row>
-    <row r="36" spans="3:10">
+        <v>3.1595510357815444</v>
+      </c>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+    </row>
+    <row r="36" spans="3:12">
       <c r="C36">
         <v>2560</v>
       </c>
@@ -2009,14 +2147,16 @@
         <v>3</v>
       </c>
       <c r="I36" s="2">
-        <v>19.207000000000001</v>
+        <v>11.291</v>
       </c>
       <c r="J36" s="2">
         <f t="shared" si="0"/>
-        <v>4.7769250793981355</v>
-      </c>
-    </row>
-    <row r="37" spans="3:10">
+        <v>8.1259764414135152</v>
+      </c>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+    </row>
+    <row r="37" spans="3:12">
       <c r="C37">
         <v>4096</v>
       </c>
@@ -2033,14 +2173,16 @@
         <v>3</v>
       </c>
       <c r="I37" s="2">
-        <v>0.48</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="J37" s="2">
         <f t="shared" si="0"/>
-        <v>1.1184810666666667</v>
-      </c>
-    </row>
-    <row r="38" spans="3:10">
+        <v>1.2936648481927711</v>
+      </c>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+    </row>
+    <row r="38" spans="3:12">
       <c r="C38">
         <v>4096</v>
       </c>
@@ -2057,14 +2199,16 @@
         <v>3</v>
       </c>
       <c r="I38" s="2">
-        <v>0.36799999999999999</v>
+        <v>0.47</v>
       </c>
       <c r="J38" s="2">
         <f t="shared" si="0"/>
-        <v>2.917776695652174</v>
-      </c>
-    </row>
-    <row r="39" spans="3:10">
+        <v>2.2845570723404256</v>
+      </c>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+    </row>
+    <row r="39" spans="3:12">
       <c r="C39">
         <v>4096</v>
       </c>
@@ -2081,14 +2225,16 @@
         <v>3</v>
       </c>
       <c r="I39" s="2">
-        <v>0.77100000000000002</v>
+        <v>0.46400000000000002</v>
       </c>
       <c r="J39" s="2">
         <f t="shared" si="0"/>
-        <v>2.7853225006485083</v>
-      </c>
-    </row>
-    <row r="40" spans="3:10">
+        <v>4.6281975172413787</v>
+      </c>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
+    </row>
+    <row r="40" spans="3:12">
       <c r="C40">
         <v>4096</v>
       </c>
@@ -2105,14 +2251,16 @@
         <v>3</v>
       </c>
       <c r="I40" s="2">
-        <v>0.65900000000000003</v>
+        <v>0.72</v>
       </c>
       <c r="J40" s="2">
         <f t="shared" si="0"/>
-        <v>6.5174010561456752</v>
-      </c>
-    </row>
-    <row r="41" spans="3:10">
+        <v>5.965232355555556</v>
+      </c>
+      <c r="K40" s="2"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="3:12">
       <c r="C41">
         <v>4096</v>
       </c>
@@ -2129,14 +2277,16 @@
         <v>3</v>
       </c>
       <c r="I41" s="2">
-        <v>61.234999999999999</v>
+        <v>35.848999999999997</v>
       </c>
       <c r="J41" s="2">
         <f t="shared" si="0"/>
-        <v>3.8357315914101417</v>
-      </c>
-    </row>
-    <row r="42" spans="3:10">
+        <v>6.551954698875841</v>
+      </c>
+      <c r="K41" s="2"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="3:12">
       <c r="C42">
         <v>1760</v>
       </c>
@@ -2156,14 +2306,16 @@
         <v>18</v>
       </c>
       <c r="I42" s="2">
-        <v>4.6420000000000003</v>
+        <v>4.2530000000000001</v>
       </c>
       <c r="J42" s="2">
         <f t="shared" si="0"/>
-        <v>9.5196815165876778</v>
-      </c>
-    </row>
-    <row r="43" spans="3:10">
+        <v>10.39039774276981</v>
+      </c>
+      <c r="K42" s="2"/>
+      <c r="L42" s="2"/>
+    </row>
+    <row r="43" spans="3:12">
       <c r="C43">
         <v>2048</v>
       </c>
@@ -2180,14 +2332,16 @@
         <v>17</v>
       </c>
       <c r="I43" s="2">
-        <v>5.851</v>
+        <v>5.6070000000000002</v>
       </c>
       <c r="J43" s="2">
         <f t="shared" si="0"/>
-        <v>10.226617819859852</v>
-      </c>
-    </row>
-    <row r="44" spans="3:10">
+        <v>10.671649877652934</v>
+      </c>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+    </row>
+    <row r="44" spans="3:12">
       <c r="C44">
         <v>2560</v>
       </c>
@@ -2204,14 +2358,16 @@
         <v>17</v>
       </c>
       <c r="I44" s="2">
-        <v>9.6609999999999996</v>
+        <v>8.7680000000000007</v>
       </c>
       <c r="J44" s="2">
         <f t="shared" si="0"/>
-        <v>9.6774306593520354</v>
-      </c>
-    </row>
-    <row r="45" spans="3:10">
+        <v>10.663054014598538</v>
+      </c>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2"/>
+    </row>
+    <row r="45" spans="3:12">
       <c r="C45" s="1">
         <v>4096</v>
       </c>
@@ -2228,22 +2384,28 @@
         <v>17</v>
       </c>
       <c r="I45" s="2">
-        <v>25.187999999999999</v>
+        <v>22.658999999999999</v>
       </c>
       <c r="J45" s="2">
         <f t="shared" si="0"/>
-        <v>9.5022932926790542</v>
-      </c>
-    </row>
-    <row r="46" spans="3:10">
+        <v>10.562856412727836</v>
+      </c>
+      <c r="K45" s="2"/>
+      <c r="L45" s="2"/>
+    </row>
+    <row r="46" spans="3:12">
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
-    </row>
-    <row r="47" spans="3:10">
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+    </row>
+    <row r="47" spans="3:12">
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
-    </row>
-    <row r="48" spans="3:10">
+      <c r="K47" s="2"/>
+      <c r="L47" s="2"/>
+    </row>
+    <row r="48" spans="3:12">
       <c r="C48">
         <v>5124</v>
       </c>
@@ -2260,14 +2422,16 @@
         <v>3</v>
       </c>
       <c r="I48" s="2">
-        <v>18.167000000000002</v>
+        <v>16.978000000000002</v>
       </c>
       <c r="J48" s="2">
         <f t="shared" si="0"/>
-        <v>9.0584490295590907</v>
-      </c>
-    </row>
-    <row r="49" spans="3:10">
+        <v>9.6928285734479918</v>
+      </c>
+      <c r="K48" s="2"/>
+      <c r="L48" s="2"/>
+    </row>
+    <row r="49" spans="3:12">
       <c r="C49">
         <v>35</v>
       </c>
@@ -2284,14 +2448,16 @@
         <v>3</v>
       </c>
       <c r="I49" s="2">
-        <v>1.038</v>
+        <v>1.0309999999999999</v>
       </c>
       <c r="J49" s="2">
         <f t="shared" si="0"/>
-        <v>1.0037595375722543</v>
-      </c>
-    </row>
-    <row r="50" spans="3:10">
+        <v>1.0105745877788554</v>
+      </c>
+      <c r="K49" s="2"/>
+      <c r="L49" s="2"/>
+    </row>
+    <row r="50" spans="3:12">
       <c r="C50">
         <v>5124</v>
       </c>
@@ -2308,14 +2474,16 @@
         <v>3</v>
       </c>
       <c r="I50" s="2">
-        <v>20.949000000000002</v>
+        <v>19.594000000000001</v>
       </c>
       <c r="J50" s="2">
         <f t="shared" si="0"/>
-        <v>9.1409440114563925</v>
-      </c>
-    </row>
-    <row r="51" spans="3:10">
+        <v>9.7730752320097984</v>
+      </c>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
+    </row>
+    <row r="51" spans="3:12">
       <c r="C51">
         <v>35</v>
       </c>
@@ -2332,14 +2500,16 @@
         <v>3</v>
       </c>
       <c r="I51" s="2">
-        <v>0.59499999999999997</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="J51" s="2">
         <f t="shared" si="0"/>
-        <v>2.0376395294117651</v>
-      </c>
-    </row>
-    <row r="52" spans="3:10">
+        <v>1.9092842834645669</v>
+      </c>
+      <c r="K51" s="2"/>
+      <c r="L51" s="2"/>
+    </row>
+    <row r="52" spans="3:12">
       <c r="C52">
         <v>5124</v>
       </c>
@@ -2356,14 +2526,16 @@
         <v>3</v>
       </c>
       <c r="I52" s="2">
-        <v>26.271999999999998</v>
+        <v>24.728999999999999</v>
       </c>
       <c r="J52" s="2">
         <f t="shared" si="0"/>
-        <v>9.1111085992691851</v>
-      </c>
-    </row>
-    <row r="53" spans="3:10">
+        <v>9.6796087637995871</v>
+      </c>
+      <c r="K52" s="2"/>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="3:12">
       <c r="C53">
         <v>35</v>
       </c>
@@ -2380,14 +2552,16 @@
         <v>3</v>
       </c>
       <c r="I53" s="2">
-        <v>1.4279999999999999</v>
+        <v>1.4219999999999999</v>
       </c>
       <c r="J53" s="2">
         <f t="shared" si="0"/>
-        <v>1.061270588235294</v>
-      </c>
-    </row>
-    <row r="54" spans="3:10">
+        <v>1.0657485232067512</v>
+      </c>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
+    </row>
+    <row r="54" spans="3:12">
       <c r="C54">
         <v>5124</v>
       </c>
@@ -2404,14 +2578,16 @@
         <v>3</v>
       </c>
       <c r="I54" s="2">
-        <v>41.914000000000001</v>
+        <v>39.119</v>
       </c>
       <c r="J54" s="2">
         <f t="shared" si="0"/>
-        <v>9.1374546020899938</v>
-      </c>
-    </row>
-    <row r="55" spans="3:10">
+        <v>9.7903134587284946</v>
+      </c>
+      <c r="K54" s="2"/>
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="3:12">
       <c r="C55">
         <v>35</v>
       </c>
@@ -2428,14 +2604,16 @@
         <v>3</v>
       </c>
       <c r="I55" s="2">
-        <v>1.1970000000000001</v>
+        <v>1.21</v>
       </c>
       <c r="J55" s="2">
         <f t="shared" si="0"/>
-        <v>2.0257235087719296</v>
-      </c>
-    </row>
-    <row r="56" spans="3:10">
+        <v>2.0039595371900827</v>
+      </c>
+      <c r="K55" s="2"/>
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="3:12">
       <c r="C56">
         <v>5124</v>
       </c>
@@ -2452,14 +2630,16 @@
         <v>3</v>
       </c>
       <c r="I56" s="2">
-        <v>33.685000000000002</v>
+        <v>47.780999999999999</v>
       </c>
       <c r="J56" s="2">
         <f t="shared" si="0"/>
-        <v>4.885404290336945</v>
-      </c>
-    </row>
-    <row r="57" spans="3:10">
+        <v>3.4441481660074094</v>
+      </c>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="3:12">
       <c r="C57">
         <v>35</v>
       </c>
@@ -2476,14 +2656,16 @@
         <v>3</v>
       </c>
       <c r="I57" s="2">
-        <v>0.36799999999999999</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="J57" s="2">
         <f t="shared" si="0"/>
-        <v>2.8312565217391303</v>
-      </c>
-    </row>
-    <row r="58" spans="3:10">
+        <v>1.9330285714285715</v>
+      </c>
+      <c r="K57" s="2"/>
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="3:12">
       <c r="C58">
         <v>5124</v>
       </c>
@@ -2500,14 +2682,16 @@
         <v>3</v>
       </c>
       <c r="I58" s="2">
-        <v>52.084000000000003</v>
+        <v>30.21</v>
       </c>
       <c r="J58" s="2">
         <f t="shared" si="0"/>
-        <v>3.6766307521695718</v>
-      </c>
-    </row>
-    <row r="59" spans="3:10">
+        <v>6.3387499535253227</v>
+      </c>
+      <c r="K58" s="2"/>
+      <c r="L58" s="2"/>
+    </row>
+    <row r="59" spans="3:12">
       <c r="C59">
         <v>35</v>
       </c>
@@ -2524,14 +2708,16 @@
         <v>3</v>
       </c>
       <c r="I59" s="2">
-        <v>0.42199999999999999</v>
+        <v>0.40400000000000003</v>
       </c>
       <c r="J59" s="2">
         <f t="shared" si="0"/>
-        <v>2.8729751658767775</v>
-      </c>
-    </row>
-    <row r="60" spans="3:10">
+        <v>3.0009790099009903</v>
+      </c>
+      <c r="K59" s="2"/>
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="3:12">
       <c r="C60">
         <v>5124</v>
       </c>
@@ -2548,14 +2734,16 @@
         <v>3</v>
       </c>
       <c r="I60" s="2">
-        <v>126.729</v>
+        <v>71.182000000000002</v>
       </c>
       <c r="J60" s="2">
         <f t="shared" si="0"/>
-        <v>1.8888103363870936</v>
-      </c>
-    </row>
-    <row r="61" spans="3:10">
+        <v>3.3627468337501054</v>
+      </c>
+      <c r="K60" s="2"/>
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="3:12">
       <c r="C61">
         <v>35</v>
       </c>
@@ -2572,14 +2760,16 @@
         <v>3</v>
       </c>
       <c r="I61" s="2">
-        <v>0.53500000000000003</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="J61" s="2">
         <f t="shared" si="0"/>
-        <v>2.8326998130841123</v>
-      </c>
-    </row>
-    <row r="62" spans="3:10">
+        <v>2.0618971428571427</v>
+      </c>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
+    </row>
+    <row r="62" spans="3:12">
       <c r="C62">
         <v>5124</v>
       </c>
@@ -2596,14 +2786,16 @@
         <v>3</v>
       </c>
       <c r="I62" s="2">
-        <v>213.83</v>
+        <v>65.885999999999996</v>
       </c>
       <c r="J62" s="2">
         <f t="shared" si="0"/>
-        <v>1.791082973352663</v>
-      </c>
-    </row>
-    <row r="63" spans="3:10">
+        <v>5.8128778828886256</v>
+      </c>
+      <c r="K62" s="2"/>
+      <c r="L62" s="2"/>
+    </row>
+    <row r="63" spans="3:12">
       <c r="C63">
         <v>35</v>
       </c>
@@ -2620,18 +2812,22 @@
         <v>3</v>
       </c>
       <c r="I63" s="2">
-        <v>0.83899999999999997</v>
+        <v>0.67300000000000004</v>
       </c>
       <c r="J63" s="2">
         <f t="shared" si="0"/>
-        <v>2.8900965911799759</v>
-      </c>
-    </row>
-    <row r="64" spans="3:10">
+        <v>3.6029584546805342</v>
+      </c>
+      <c r="K63" s="2"/>
+      <c r="L63" s="2"/>
+    </row>
+    <row r="64" spans="3:12">
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
-    </row>
-    <row r="65" spans="3:10">
+      <c r="K64" s="2"/>
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="3:12">
       <c r="C65">
         <v>7680</v>
       </c>
@@ -2648,14 +2844,16 @@
         <v>3</v>
       </c>
       <c r="I65" s="2">
-        <v>0.877</v>
+        <v>0.879</v>
       </c>
       <c r="J65" s="2">
         <f t="shared" si="0"/>
-        <v>0.71738380843785632</v>
-      </c>
-    </row>
-    <row r="66" spans="3:10">
+        <v>0.71575153583617745</v>
+      </c>
+      <c r="K65" s="2"/>
+      <c r="L65" s="2"/>
+    </row>
+    <row r="66" spans="3:12">
       <c r="C66">
         <v>7680</v>
       </c>
@@ -2672,14 +2870,16 @@
         <v>3</v>
       </c>
       <c r="I66" s="2">
-        <v>0.41199999999999998</v>
+        <v>0.33100000000000002</v>
       </c>
       <c r="J66" s="2">
         <f t="shared" si="0"/>
-        <v>3.0541048543689322</v>
-      </c>
-    </row>
-    <row r="67" spans="3:10">
+        <v>3.8014839879154079</v>
+      </c>
+      <c r="K66" s="2"/>
+      <c r="L66" s="2"/>
+    </row>
+    <row r="67" spans="3:12">
       <c r="C67">
         <v>7680</v>
       </c>
@@ -2696,14 +2896,16 @@
         <v>3</v>
       </c>
       <c r="I67" s="2">
-        <v>0.42399999999999999</v>
+        <v>0.45</v>
       </c>
       <c r="J67" s="2">
         <f t="shared" ref="J67:J83" si="1">(2*C67*D67*E67)/(I67/1000)/10^12</f>
-        <v>5.9353358490566039</v>
-      </c>
-    </row>
-    <row r="68" spans="3:10">
+        <v>5.5924053333333328</v>
+      </c>
+      <c r="K67" s="2"/>
+      <c r="L67" s="2"/>
+    </row>
+    <row r="68" spans="3:12">
       <c r="C68">
         <v>7680</v>
       </c>
@@ -2720,14 +2922,16 @@
         <v>3</v>
       </c>
       <c r="I68" s="2">
-        <v>0.65200000000000002</v>
+        <v>0.73699999999999999</v>
       </c>
       <c r="J68" s="2">
         <f t="shared" si="1"/>
-        <v>7.7195779141104293</v>
-      </c>
-    </row>
-    <row r="69" spans="3:10">
+        <v>6.8292602442333781</v>
+      </c>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+    </row>
+    <row r="69" spans="3:12">
       <c r="C69">
         <v>7680</v>
       </c>
@@ -2744,14 +2948,16 @@
         <v>3</v>
       </c>
       <c r="I69" s="2">
-        <v>0.83699999999999997</v>
+        <v>0.53700000000000003</v>
       </c>
       <c r="J69" s="2">
         <f t="shared" si="1"/>
-        <v>0.75166738351254481</v>
-      </c>
-    </row>
-    <row r="70" spans="3:10">
+        <v>1.1715932960893856</v>
+      </c>
+      <c r="K69" s="2"/>
+      <c r="L69" s="2"/>
+    </row>
+    <row r="70" spans="3:12">
       <c r="C70">
         <v>7680</v>
       </c>
@@ -2768,14 +2974,16 @@
         <v>3</v>
       </c>
       <c r="I70" s="2">
-        <v>0.67800000000000005</v>
+        <v>0.69799999999999995</v>
       </c>
       <c r="J70" s="2">
         <f t="shared" si="1"/>
-        <v>1.8558867256637168</v>
-      </c>
-    </row>
-    <row r="71" spans="3:10">
+        <v>1.8027094555873926</v>
+      </c>
+      <c r="K70" s="2"/>
+      <c r="L70" s="2"/>
+    </row>
+    <row r="71" spans="3:12">
       <c r="C71">
         <v>7680</v>
       </c>
@@ -2792,14 +3000,16 @@
         <v>3</v>
       </c>
       <c r="I71" s="2">
-        <v>1.0349999999999999</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="J71" s="2">
         <f t="shared" si="1"/>
-        <v>2.4314805797101449</v>
-      </c>
-    </row>
-    <row r="72" spans="3:10">
+        <v>3.5696204255319151</v>
+      </c>
+      <c r="K71" s="2"/>
+      <c r="L71" s="2"/>
+    </row>
+    <row r="72" spans="3:12">
       <c r="C72">
         <v>7680</v>
       </c>
@@ -2816,14 +3026,16 @@
         <v>3</v>
       </c>
       <c r="I72" s="2">
-        <v>1.93</v>
+        <v>1.615</v>
       </c>
       <c r="J72" s="2">
         <f t="shared" si="1"/>
-        <v>2.6078574093264253</v>
-      </c>
-    </row>
-    <row r="73" spans="3:10">
+        <v>3.1165107120743039</v>
+      </c>
+      <c r="K72" s="2"/>
+      <c r="L72" s="2"/>
+    </row>
+    <row r="73" spans="3:12">
       <c r="C73">
         <f>3*1024</f>
         <v>3072</v>
@@ -2841,14 +3053,16 @@
         <v>3</v>
       </c>
       <c r="I73" s="2">
-        <v>7.6999999999999999E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="J73" s="2">
         <f t="shared" si="1"/>
-        <v>1.3073155324675325</v>
-      </c>
-    </row>
-    <row r="74" spans="3:10">
+        <v>1.2905550769230769</v>
+      </c>
+      <c r="K73" s="2"/>
+      <c r="L73" s="2"/>
+    </row>
+    <row r="74" spans="3:12">
       <c r="C74">
         <f t="shared" ref="C74:C80" si="2">3*1024</f>
         <v>3072</v>
@@ -2872,8 +3086,10 @@
         <f t="shared" si="1"/>
         <v>1.7506660173913042</v>
       </c>
-    </row>
-    <row r="75" spans="3:10">
+      <c r="K74" s="2"/>
+      <c r="L74" s="2"/>
+    </row>
+    <row r="75" spans="3:12">
       <c r="C75">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2891,14 +3107,16 @@
         <v>3</v>
       </c>
       <c r="I75" s="2">
-        <v>0.104</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="J75" s="2">
         <f t="shared" si="1"/>
-        <v>3.871665230769231</v>
-      </c>
-    </row>
-    <row r="76" spans="3:10">
+        <v>3.0274675488721803</v>
+      </c>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+    </row>
+    <row r="76" spans="3:12">
       <c r="C76">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2916,14 +3134,16 @@
         <v>3</v>
       </c>
       <c r="I76" s="2">
-        <v>0.105</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="J76" s="2">
         <f t="shared" si="1"/>
-        <v>7.6695844571428573</v>
-      </c>
-    </row>
-    <row r="77" spans="3:10">
+        <v>6.0549350977443606</v>
+      </c>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+    </row>
+    <row r="77" spans="3:12">
       <c r="C77">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2941,14 +3161,16 @@
         <v>3</v>
       </c>
       <c r="I77" s="2">
-        <v>0.129</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="J77" s="2">
         <f t="shared" si="1"/>
-        <v>0.78033562790697686</v>
-      </c>
-    </row>
-    <row r="78" spans="3:10">
+        <v>1.0824010322580646</v>
+      </c>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+    </row>
+    <row r="78" spans="3:12">
       <c r="C78">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2966,14 +3188,16 @@
         <v>3</v>
       </c>
       <c r="I78" s="2">
-        <v>8.4000000000000005E-2</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="J78" s="2">
         <f t="shared" si="1"/>
-        <v>2.3967451428571427</v>
-      </c>
-    </row>
-    <row r="79" spans="3:10">
+        <v>1.491308088888889</v>
+      </c>
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+    </row>
+    <row r="79" spans="3:12">
       <c r="C79">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -2991,14 +3215,16 @@
         <v>3</v>
       </c>
       <c r="I79" s="2">
-        <v>0.13200000000000001</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="J79" s="2">
         <f t="shared" si="1"/>
-        <v>3.0504029090909088</v>
-      </c>
-    </row>
-    <row r="80" spans="3:10">
+        <v>2.9606851764705886</v>
+      </c>
+      <c r="K79" s="2"/>
+      <c r="L79" s="2"/>
+    </row>
+    <row r="80" spans="3:12">
       <c r="C80">
         <f t="shared" si="2"/>
         <v>3072</v>
@@ -3016,18 +3242,22 @@
         <v>3</v>
       </c>
       <c r="I80" s="2">
-        <v>0.28100000000000003</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="J80" s="2">
         <f t="shared" si="1"/>
-        <v>2.8658589608540916</v>
-      </c>
-    </row>
-    <row r="81" spans="1:29">
+        <v>6.0097490149253732</v>
+      </c>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+    </row>
+    <row r="81" spans="1:31">
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
-    </row>
-    <row r="82" spans="1:29">
+      <c r="K81" s="2"/>
+      <c r="L81" s="2"/>
+    </row>
+    <row r="82" spans="1:31">
       <c r="C82">
         <v>3072</v>
       </c>
@@ -3044,14 +3274,16 @@
         <v>17</v>
       </c>
       <c r="I82" s="2">
-        <v>5.1029999999999998</v>
+        <v>4.9269999999999996</v>
       </c>
       <c r="J82" s="2">
         <f t="shared" si="1"/>
-        <v>9.1665638565549692</v>
-      </c>
-    </row>
-    <row r="83" spans="1:29">
+        <v>9.4940075827075301</v>
+      </c>
+      <c r="K82" s="2"/>
+      <c r="L82" s="2"/>
+    </row>
+    <row r="83" spans="1:31">
       <c r="C83">
         <v>7680</v>
       </c>
@@ -3068,22 +3300,24 @@
         <v>17</v>
       </c>
       <c r="I83" s="2">
-        <v>22.809000000000001</v>
+        <v>20.986000000000001</v>
       </c>
       <c r="J83" s="2">
         <f t="shared" si="1"/>
-        <v>9.4489758253321057</v>
-      </c>
-    </row>
-    <row r="87" spans="1:29">
+        <v>10.269784122748497</v>
+      </c>
+      <c r="K83" s="2"/>
+      <c r="L83" s="2"/>
+    </row>
+    <row r="87" spans="1:31">
       <c r="J87" s="3"/>
     </row>
-    <row r="89" spans="1:29">
+    <row r="89" spans="1:31">
       <c r="A89" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:29">
+    <row r="90" spans="1:31">
       <c r="C90" t="s">
         <v>7</v>
       </c>
@@ -3148,7 +3382,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="91" spans="1:29">
+    <row r="91" spans="1:31">
       <c r="C91">
         <v>700</v>
       </c>
@@ -3183,44 +3417,44 @@
         <v>2</v>
       </c>
       <c r="N91" s="2">
-        <v>0.13400000000000001</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="O91" s="2" t="s">
         <v>60</v>
       </c>
       <c r="P91" s="2">
-        <v>0.28199999999999997</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="R91" s="4">
-        <f>(D91-H91+1+2*J91)/L91</f>
+        <f t="shared" ref="R91:R126" si="3">(D91-H91+1+2*J91)/L91</f>
         <v>78.5</v>
       </c>
       <c r="S91" s="4">
-        <f>(C91-I91+1+2*K91)/M91</f>
+        <f t="shared" ref="S91:S126" si="4">(C91-I91+1+2*K91)/M91</f>
         <v>340.5</v>
       </c>
       <c r="T91" s="2">
         <f>N91+P91</f>
-        <v>0.41599999999999998</v>
+        <v>0.41200000000000003</v>
       </c>
       <c r="U91" s="2">
         <f>(2*$R91*$S91*$F91*$G91*$E91*$H91*$I91)/(N91/1000)/10^12</f>
-        <v>5.1064835820895516</v>
+        <v>5.1838545454545448</v>
       </c>
       <c r="V91" s="2" t="s">
         <v>60</v>
       </c>
       <c r="W91" s="2">
         <f>(2*$R91*$S91*$F91*$G91*$E91*$H91*$I91)/(P91/1000)/10^12</f>
-        <v>2.4264851063829789</v>
+        <v>2.4438171428571427</v>
       </c>
       <c r="X91" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA91" s="2"/>
-      <c r="AC91" s="2"/>
-    </row>
-    <row r="92" spans="1:29">
+      <c r="AE91" s="2"/>
+    </row>
+    <row r="92" spans="1:31">
       <c r="C92">
         <v>700</v>
       </c>
@@ -3255,44 +3489,44 @@
         <v>2</v>
       </c>
       <c r="N92" s="2">
-        <v>0.252</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="O92" s="2" t="s">
         <v>60</v>
       </c>
       <c r="P92" s="2">
-        <v>0.52900000000000003</v>
+        <v>0.51500000000000001</v>
       </c>
       <c r="R92" s="4">
-        <f t="shared" ref="R92:R126" si="3">(D92-H92+1+2*J92)/L92</f>
+        <f t="shared" si="3"/>
         <v>78.5</v>
       </c>
       <c r="S92" s="4">
-        <f t="shared" ref="S92:S126" si="4">(C92-I92+1+2*K92)/M92</f>
+        <f t="shared" si="4"/>
         <v>340.5</v>
       </c>
       <c r="T92" s="2">
         <f>N92+P92</f>
-        <v>0.78100000000000003</v>
+        <v>0.746</v>
       </c>
       <c r="U92" s="2">
         <f t="shared" ref="U92:U126" si="5">(2*$R92*$S92*$F92*$G92*$E92*$H92*$I92)/(N92/1000)/10^12</f>
-        <v>5.4307047619047619</v>
+        <v>5.9244051948051943</v>
       </c>
       <c r="V92" s="2" t="s">
         <v>60</v>
       </c>
       <c r="W92" s="2">
         <f t="shared" ref="W92:W126" si="6">(2*$R92*$S92*$F92*$G92*$E92*$H92*$I92)/(P92/1000)/10^12</f>
-        <v>2.5870275992438558</v>
+        <v>2.6573545631067961</v>
       </c>
       <c r="X92" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA92" s="2"/>
-      <c r="AC92" s="2"/>
-    </row>
-    <row r="93" spans="1:29">
+      <c r="AE92" s="2"/>
+    </row>
+    <row r="93" spans="1:31">
       <c r="C93">
         <v>700</v>
       </c>
@@ -3327,13 +3561,13 @@
         <v>2</v>
       </c>
       <c r="N93" s="2">
-        <v>0.44800000000000001</v>
+        <v>0.41</v>
       </c>
       <c r="O93" s="2" t="s">
         <v>60</v>
       </c>
       <c r="P93" s="2">
-        <v>0.99099999999999999</v>
+        <v>0.98699999999999999</v>
       </c>
       <c r="R93" s="4">
         <f t="shared" si="3"/>
@@ -3345,26 +3579,26 @@
       </c>
       <c r="T93" s="2">
         <f>N93+P93</f>
-        <v>1.4390000000000001</v>
+        <v>1.397</v>
       </c>
       <c r="U93" s="2">
         <f t="shared" si="5"/>
-        <v>6.1095428571428574</v>
+        <v>6.6757931707317066</v>
       </c>
       <c r="V93" s="2" t="s">
         <v>60</v>
       </c>
       <c r="W93" s="2">
         <f t="shared" si="6"/>
-        <v>2.7619325933400609</v>
+        <v>2.7731258358662614</v>
       </c>
       <c r="X93" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA93" s="2"/>
-      <c r="AC93" s="2"/>
-    </row>
-    <row r="94" spans="1:29">
+      <c r="AE93" s="2"/>
+    </row>
+    <row r="94" spans="1:31">
       <c r="C94">
         <v>700</v>
       </c>
@@ -3399,13 +3633,13 @@
         <v>2</v>
       </c>
       <c r="N94" s="2">
-        <v>0.82599999999999996</v>
+        <v>0.82499999999999996</v>
       </c>
       <c r="O94" s="2" t="s">
         <v>60</v>
       </c>
       <c r="P94" s="2">
-        <v>2.1549999999999998</v>
+        <v>2.1349999999999998</v>
       </c>
       <c r="R94" s="4">
         <f t="shared" si="3"/>
@@ -3417,26 +3651,26 @@
       </c>
       <c r="T94" s="2">
         <f>N94+P94</f>
-        <v>2.9809999999999999</v>
+        <v>2.96</v>
       </c>
       <c r="U94" s="2">
         <f t="shared" si="5"/>
-        <v>6.627300726392253</v>
+        <v>6.6353338181818184</v>
       </c>
       <c r="V94" s="2" t="s">
         <v>60</v>
       </c>
       <c r="W94" s="2">
         <f t="shared" si="6"/>
-        <v>2.5402090023201862</v>
+        <v>2.5640048711943799</v>
       </c>
       <c r="X94" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA94" s="2"/>
-      <c r="AC94" s="2"/>
-    </row>
-    <row r="95" spans="1:29">
+      <c r="AE94" s="2"/>
+    </row>
+    <row r="95" spans="1:31">
       <c r="C95">
         <v>341</v>
       </c>
@@ -3471,13 +3705,13 @@
         <v>2</v>
       </c>
       <c r="N95" s="2">
-        <v>0.38</v>
+        <v>0.378</v>
       </c>
       <c r="O95" s="2">
-        <v>1.476</v>
+        <v>1.5229999999999999</v>
       </c>
       <c r="P95" s="2">
-        <v>0.45300000000000001</v>
+        <v>0.45100000000000001</v>
       </c>
       <c r="R95" s="4">
         <f t="shared" si="3"/>
@@ -3489,27 +3723,27 @@
       </c>
       <c r="T95" s="2">
         <f>N95+O95+P95</f>
-        <v>2.3089999999999997</v>
+        <v>2.3519999999999999</v>
       </c>
       <c r="U95" s="2">
         <f t="shared" si="5"/>
-        <v>6.7098947368421049</v>
+        <v>6.7453968253968251</v>
       </c>
       <c r="V95" s="2">
         <f t="shared" ref="V95:V126" si="7">(2*$R95*$S95*$F95*$G95*$E95*$H95*$I95)/(O95/1000)/10^12</f>
-        <v>1.727479674796748</v>
+        <v>1.6741694024950757</v>
       </c>
       <c r="W95" s="2">
         <f t="shared" si="6"/>
-        <v>5.628609271523179</v>
+        <v>5.6535698447893568</v>
       </c>
       <c r="X95" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA95" s="2"/>
-      <c r="AC95" s="2"/>
-    </row>
-    <row r="96" spans="1:29">
+      <c r="AE95" s="2"/>
+    </row>
+    <row r="96" spans="1:31">
       <c r="C96">
         <v>341</v>
       </c>
@@ -3544,13 +3778,13 @@
         <v>2</v>
       </c>
       <c r="N96" s="2">
-        <v>0.64500000000000002</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="O96" s="2">
-        <v>2.9780000000000002</v>
+        <v>2.895</v>
       </c>
       <c r="P96" s="2">
-        <v>0.90100000000000002</v>
+        <v>0.89400000000000002</v>
       </c>
       <c r="R96" s="4">
         <f t="shared" si="3"/>
@@ -3562,27 +3796,27 @@
       </c>
       <c r="T96" s="2">
         <f t="shared" ref="T96:T98" si="8">N96+O96+P96</f>
-        <v>4.524</v>
+        <v>4.4370000000000003</v>
       </c>
       <c r="U96" s="2">
         <f t="shared" si="5"/>
-        <v>7.9062325581395339</v>
+        <v>7.8696296296296291</v>
       </c>
       <c r="V96" s="2">
         <f t="shared" si="7"/>
-        <v>1.7123975822699797</v>
+        <v>1.7614922279792746</v>
       </c>
       <c r="W96" s="2">
         <f t="shared" si="6"/>
-        <v>5.6598446170921202</v>
+        <v>5.7041610738255031</v>
       </c>
       <c r="X96" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA96" s="2"/>
-      <c r="AC96" s="2"/>
-    </row>
-    <row r="97" spans="3:29">
+      <c r="AE96" s="2"/>
+    </row>
+    <row r="97" spans="3:31">
       <c r="C97">
         <v>341</v>
       </c>
@@ -3617,13 +3851,13 @@
         <v>2</v>
       </c>
       <c r="N97" s="2">
-        <v>1.319</v>
+        <v>1.3169999999999999</v>
       </c>
       <c r="O97" s="2">
-        <v>5.7359999999999998</v>
+        <v>5.6870000000000003</v>
       </c>
       <c r="P97" s="2">
-        <v>1.732</v>
+        <v>1.726</v>
       </c>
       <c r="R97" s="4">
         <f t="shared" si="3"/>
@@ -3635,27 +3869,27 @@
       </c>
       <c r="T97" s="2">
         <f t="shared" si="8"/>
-        <v>8.786999999999999</v>
+        <v>8.73</v>
       </c>
       <c r="U97" s="2">
         <f t="shared" si="5"/>
-        <v>7.7324033358605009</v>
+        <v>7.7441457858769933</v>
       </c>
       <c r="V97" s="2">
         <f t="shared" si="7"/>
-        <v>1.7780753138075316</v>
+        <v>1.7933954633374363</v>
       </c>
       <c r="W97" s="2">
         <f t="shared" si="6"/>
-        <v>5.8885912240184757</v>
+        <v>5.9090614136732338</v>
       </c>
       <c r="X97" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA97" s="2"/>
-      <c r="AC97" s="2"/>
-    </row>
-    <row r="98" spans="3:29">
+      <c r="AE97" s="2"/>
+    </row>
+    <row r="98" spans="3:31">
       <c r="C98">
         <v>341</v>
       </c>
@@ -3690,13 +3924,13 @@
         <v>2</v>
       </c>
       <c r="N98" s="2">
-        <v>2.6920000000000002</v>
+        <v>2.7389999999999999</v>
       </c>
       <c r="O98" s="2">
-        <v>11.332000000000001</v>
+        <v>11.247999999999999</v>
       </c>
       <c r="P98" s="2">
-        <v>3.3959999999999999</v>
+        <v>3.4060000000000001</v>
       </c>
       <c r="R98" s="4">
         <f t="shared" si="3"/>
@@ -3708,27 +3942,27 @@
       </c>
       <c r="T98" s="2">
         <f t="shared" si="8"/>
-        <v>17.420000000000002</v>
+        <v>17.392999999999997</v>
       </c>
       <c r="U98" s="2">
         <f t="shared" si="5"/>
-        <v>7.5772956909361051</v>
+        <v>7.4472727272727282</v>
       </c>
       <c r="V98" s="2">
         <f t="shared" si="7"/>
-        <v>1.8000423579244618</v>
+        <v>1.81348506401138</v>
       </c>
       <c r="W98" s="2">
         <f t="shared" si="6"/>
-        <v>6.0065017667844529</v>
+        <v>5.9888667058132707</v>
       </c>
       <c r="X98" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA98" s="2"/>
-      <c r="AC98" s="2"/>
-    </row>
-    <row r="99" spans="3:29">
+      <c r="AE98" s="2"/>
+    </row>
+    <row r="99" spans="3:31">
       <c r="C99">
         <v>480</v>
       </c>
@@ -3765,11 +3999,11 @@
       <c r="N99" s="2">
         <v>0.11899999999999999</v>
       </c>
-      <c r="O99" s="2">
-        <v>0.36099999999999999</v>
+      <c r="O99" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="P99" s="2">
-        <v>0.41199999999999998</v>
+        <v>0.40600000000000003</v>
       </c>
       <c r="R99" s="4">
         <f t="shared" si="3"/>
@@ -3781,27 +4015,26 @@
       </c>
       <c r="T99" s="2">
         <f>N99+P99</f>
-        <v>0.53099999999999992</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="U99" s="2">
         <f t="shared" si="5"/>
         <v>0.89217075630252107</v>
       </c>
-      <c r="V99" s="2">
-        <f t="shared" si="7"/>
-        <v>0.29409506925207757</v>
+      <c r="V99" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="W99" s="2">
         <f t="shared" si="6"/>
-        <v>0.25769009708737867</v>
+        <v>0.26149832512315269</v>
       </c>
       <c r="X99" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA99" s="2"/>
-      <c r="AC99" s="2"/>
-    </row>
-    <row r="100" spans="3:29">
+      <c r="AE99" s="2"/>
+    </row>
+    <row r="100" spans="3:31">
       <c r="C100">
         <v>240</v>
       </c>
@@ -3836,13 +4069,13 @@
         <v>1</v>
       </c>
       <c r="N100" s="2">
-        <v>0.14199999999999999</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="O100" s="2">
-        <v>0.16900000000000001</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="P100" s="2">
-        <v>0.502</v>
+        <v>0.495</v>
       </c>
       <c r="R100" s="4">
         <f t="shared" si="3"/>
@@ -3854,27 +4087,27 @@
       </c>
       <c r="T100" s="2">
         <f>N100+O100+P100</f>
-        <v>0.81299999999999994</v>
+        <v>0.80200000000000005</v>
       </c>
       <c r="U100" s="2">
         <f t="shared" si="5"/>
-        <v>5.9813138028169019</v>
+        <v>6.0667611428571426</v>
       </c>
       <c r="V100" s="2">
         <f t="shared" si="7"/>
-        <v>5.0257192899408283</v>
+        <v>5.0859075449101789</v>
       </c>
       <c r="W100" s="2">
         <f t="shared" si="6"/>
-        <v>1.6919254183266934</v>
+        <v>1.7158516363636365</v>
       </c>
       <c r="X100" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA100" s="2"/>
-      <c r="AC100" s="2"/>
-    </row>
-    <row r="101" spans="3:29">
+      <c r="AE100" s="2"/>
+    </row>
+    <row r="101" spans="3:31">
       <c r="C101">
         <v>120</v>
       </c>
@@ -3909,13 +4142,13 @@
         <v>1</v>
       </c>
       <c r="N101" s="2">
-        <v>0.11600000000000001</v>
+        <v>0.114</v>
       </c>
       <c r="O101" s="2">
-        <v>8.4000000000000005E-2</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="P101" s="2">
-        <v>0.32900000000000001</v>
+        <v>0.33200000000000002</v>
       </c>
       <c r="R101" s="4">
         <f t="shared" si="3"/>
@@ -3927,27 +4160,27 @@
       </c>
       <c r="T101" s="2">
         <f t="shared" ref="T101:T102" si="9">N101+O101+P101</f>
-        <v>0.52900000000000003</v>
+        <v>0.53100000000000003</v>
       </c>
       <c r="U101" s="2">
         <f t="shared" si="5"/>
-        <v>7.3219531034482754</v>
+        <v>7.4504084210526305</v>
       </c>
       <c r="V101" s="2">
         <f t="shared" si="7"/>
-        <v>10.111268571428571</v>
+        <v>9.9923124705882351</v>
       </c>
       <c r="W101" s="2">
         <f t="shared" si="6"/>
-        <v>2.5816004863221882</v>
+        <v>2.5582727710843374</v>
       </c>
       <c r="X101" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA101" s="2"/>
-      <c r="AC101" s="2"/>
-    </row>
-    <row r="102" spans="3:29">
+      <c r="AE101" s="2"/>
+    </row>
+    <row r="102" spans="3:31">
       <c r="C102">
         <v>60</v>
       </c>
@@ -3982,13 +4215,13 @@
         <v>1</v>
       </c>
       <c r="N102" s="2">
-        <v>0.08</v>
+        <v>8.2000000000000003E-2</v>
       </c>
       <c r="O102" s="2">
-        <v>7.0000000000000007E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="P102" s="2">
-        <v>0.18</v>
+        <v>0.183</v>
       </c>
       <c r="R102" s="4">
         <f t="shared" si="3"/>
@@ -4000,27 +4233,27 @@
       </c>
       <c r="T102" s="2">
         <f t="shared" si="9"/>
-        <v>0.33</v>
+        <v>0.33599999999999997</v>
       </c>
       <c r="U102" s="2">
         <f t="shared" si="5"/>
-        <v>10.616832</v>
+        <v>10.357884878048781</v>
       </c>
       <c r="V102" s="2">
         <f t="shared" si="7"/>
-        <v>12.133522285714285</v>
+        <v>11.962627605633804</v>
       </c>
       <c r="W102" s="2">
         <f t="shared" si="6"/>
-        <v>4.7185920000000001</v>
+        <v>4.6412380327868847</v>
       </c>
       <c r="X102" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AA102" s="2"/>
-      <c r="AC102" s="2"/>
-    </row>
-    <row r="103" spans="3:29">
+      <c r="AE102" s="2"/>
+    </row>
+    <row r="103" spans="3:31">
       <c r="C103">
         <v>108</v>
       </c>
@@ -4055,13 +4288,13 @@
         <v>2</v>
       </c>
       <c r="N103" s="2">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="O103" s="2">
-        <v>7.6999999999999999E-2</v>
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="O103" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="P103" s="2">
-        <v>0.1</v>
+        <v>0.10199999999999999</v>
       </c>
       <c r="R103" s="4">
         <f t="shared" si="3"/>
@@ -4073,27 +4306,26 @@
       </c>
       <c r="T103" s="2">
         <f>N103+P103</f>
-        <v>0.13600000000000001</v>
+        <v>0.13899999999999998</v>
       </c>
       <c r="U103" s="2">
         <f t="shared" si="5"/>
-        <v>2.2394880000000006</v>
-      </c>
-      <c r="V103" s="2">
-        <f t="shared" si="7"/>
-        <v>1.0470333506493505</v>
+        <v>2.1789612972972972</v>
+      </c>
+      <c r="V103" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="W103" s="2">
         <f t="shared" si="6"/>
-        <v>0.80621567999999999</v>
+        <v>0.79040752941176473</v>
       </c>
       <c r="X103" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA103" s="2"/>
-      <c r="AC103" s="2"/>
-    </row>
-    <row r="104" spans="3:29">
+      <c r="AE103" s="2"/>
+    </row>
+    <row r="104" spans="3:31">
       <c r="C104">
         <v>54</v>
       </c>
@@ -4128,13 +4360,13 @@
         <v>1</v>
       </c>
       <c r="N104" s="2">
-        <v>0.159</v>
+        <v>0.16</v>
       </c>
       <c r="O104" s="2">
         <v>0.16300000000000001</v>
       </c>
       <c r="P104" s="2">
-        <v>0.307</v>
+        <v>0.311</v>
       </c>
       <c r="R104" s="4">
         <f t="shared" si="3"/>
@@ -4146,11 +4378,11 @@
       </c>
       <c r="T104" s="2">
         <f>N104+O104+P104</f>
-        <v>0.629</v>
+        <v>0.63400000000000001</v>
       </c>
       <c r="U104" s="2">
         <f t="shared" si="5"/>
-        <v>10.81714958490566</v>
+        <v>10.749542399999999</v>
       </c>
       <c r="V104" s="2">
         <f t="shared" si="7"/>
@@ -4158,15 +4390,15 @@
       </c>
       <c r="W104" s="2">
         <f t="shared" si="6"/>
-        <v>5.6023673745928342</v>
+        <v>5.5303112025723467</v>
       </c>
       <c r="X104" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AA104" s="2"/>
-      <c r="AC104" s="2"/>
-    </row>
-    <row r="105" spans="3:29">
+      <c r="AE104" s="2"/>
+    </row>
+    <row r="105" spans="3:31">
       <c r="C105">
         <v>27</v>
       </c>
@@ -4201,13 +4433,13 @@
         <v>1</v>
       </c>
       <c r="N105" s="2">
-        <v>0.13</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="O105" s="2">
-        <v>0.13300000000000001</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="P105" s="2">
-        <v>0.23400000000000001</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="R105" s="4">
         <f t="shared" si="3"/>
@@ -4223,23 +4455,23 @@
       </c>
       <c r="U105" s="2">
         <f t="shared" si="5"/>
-        <v>13.230206030769228</v>
+        <v>13.029748363636363</v>
       </c>
       <c r="V105" s="2">
         <f t="shared" si="7"/>
-        <v>12.931780330827067</v>
+        <v>13.029748363636363</v>
       </c>
       <c r="W105" s="2">
         <f t="shared" si="6"/>
-        <v>7.3501144615384613</v>
+        <v>7.3816600171673805</v>
       </c>
       <c r="X105" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AA105" s="2"/>
-      <c r="AC105" s="2"/>
-    </row>
-    <row r="106" spans="3:29">
+      <c r="AE105" s="2"/>
+    </row>
+    <row r="106" spans="3:31">
       <c r="C106">
         <v>14</v>
       </c>
@@ -4274,13 +4506,13 @@
         <v>1</v>
       </c>
       <c r="N106" s="2">
-        <v>7.9000000000000001E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="O106" s="2">
-        <v>7.3999999999999996E-2</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="P106" s="2">
-        <v>0.157</v>
+        <v>0.153</v>
       </c>
       <c r="R106" s="4">
         <f t="shared" si="3"/>
@@ -4292,27 +4524,27 @@
       </c>
       <c r="T106" s="2">
         <f t="shared" si="10"/>
-        <v>0.31</v>
+        <v>0.30299999999999999</v>
       </c>
       <c r="U106" s="2">
         <f t="shared" si="5"/>
-        <v>11.706886481012658</v>
+        <v>12.010961454545455</v>
       </c>
       <c r="V106" s="2">
         <f t="shared" si="7"/>
-        <v>12.497892324324324</v>
+        <v>12.669096328767123</v>
       </c>
       <c r="W106" s="2">
         <f t="shared" si="6"/>
-        <v>5.8907263184713381</v>
+        <v>6.0447322352941173</v>
       </c>
       <c r="X106" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AA106" s="2"/>
-      <c r="AC106" s="2"/>
-    </row>
-    <row r="107" spans="3:29">
+      <c r="AE106" s="2"/>
+    </row>
+    <row r="107" spans="3:31">
       <c r="C107">
         <v>7</v>
       </c>
@@ -4347,13 +4579,13 @@
         <v>1</v>
       </c>
       <c r="N107" s="2">
-        <v>0.19</v>
+        <v>0.187</v>
       </c>
       <c r="O107" s="2">
-        <v>0.20200000000000001</v>
+        <v>0.19700000000000001</v>
       </c>
       <c r="P107" s="2">
-        <v>0.28399999999999997</v>
+        <v>0.28299999999999997</v>
       </c>
       <c r="R107" s="4">
         <f t="shared" si="3"/>
@@ -4365,27 +4597,27 @@
       </c>
       <c r="T107" s="2">
         <f t="shared" si="10"/>
-        <v>0.67599999999999993</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="U107" s="2">
         <f t="shared" si="5"/>
-        <v>4.8676001684210526</v>
+        <v>4.9456900106951878</v>
       </c>
       <c r="V107" s="2">
         <f t="shared" si="7"/>
-        <v>4.5784358019801985</v>
+        <v>4.6946397563451772</v>
       </c>
       <c r="W107" s="2">
         <f t="shared" si="6"/>
-        <v>3.2564930704225357</v>
+        <v>3.2680001130742049</v>
       </c>
       <c r="X107" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AA107" s="2"/>
-      <c r="AC107" s="2"/>
-    </row>
-    <row r="108" spans="3:29">
+      <c r="AE107" s="2"/>
+    </row>
+    <row r="108" spans="3:31">
       <c r="C108">
         <v>224</v>
       </c>
@@ -4420,13 +4652,13 @@
         <v>1</v>
       </c>
       <c r="N108" s="2">
-        <v>0.39300000000000002</v>
+        <v>0.39800000000000002</v>
       </c>
       <c r="O108" s="2" t="s">
         <v>60</v>
       </c>
       <c r="P108" s="2">
-        <v>1.6060000000000001</v>
+        <v>1.611</v>
       </c>
       <c r="R108" s="4">
         <f t="shared" si="3"/>
@@ -4438,26 +4670,26 @@
       </c>
       <c r="T108" s="2">
         <f>N108+P108</f>
-        <v>1.9990000000000001</v>
+        <v>2.0089999999999999</v>
       </c>
       <c r="U108" s="2">
         <f t="shared" si="5"/>
-        <v>3.5299390534351143</v>
+        <v>3.4855930854271353</v>
       </c>
       <c r="V108" s="2" t="s">
         <v>60</v>
       </c>
       <c r="W108" s="2">
         <f t="shared" si="6"/>
-        <v>0.86380202241594017</v>
+        <v>0.86112107262569837</v>
       </c>
       <c r="X108" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA108" s="2"/>
-      <c r="AC108" s="2"/>
-    </row>
-    <row r="109" spans="3:29">
+      <c r="AE108" s="2"/>
+    </row>
+    <row r="109" spans="3:31">
       <c r="C109">
         <v>112</v>
       </c>
@@ -4492,13 +4724,13 @@
         <v>1</v>
       </c>
       <c r="N109" s="2">
-        <v>0.98</v>
+        <v>0.97699999999999998</v>
       </c>
       <c r="O109" s="2">
-        <v>0.89200000000000002</v>
+        <v>0.88900000000000001</v>
       </c>
       <c r="P109" s="2">
-        <v>1.8420000000000001</v>
+        <v>1.847</v>
       </c>
       <c r="R109" s="4">
         <f t="shared" si="3"/>
@@ -4510,27 +4742,27 @@
       </c>
       <c r="T109" s="2">
         <f>N109+O109+P109</f>
-        <v>3.714</v>
+        <v>3.7130000000000001</v>
       </c>
       <c r="U109" s="2">
         <f t="shared" si="5"/>
-        <v>15.099494399999999</v>
+        <v>15.145859275332651</v>
       </c>
       <c r="V109" s="2">
         <f t="shared" si="7"/>
-        <v>16.58913061883408</v>
+        <v>16.645111937007872</v>
       </c>
       <c r="W109" s="2">
         <f t="shared" si="6"/>
-        <v>8.0333900716612376</v>
+        <v>8.0116429409853822</v>
       </c>
       <c r="X109" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AA109" s="2"/>
-      <c r="AC109" s="2"/>
-    </row>
-    <row r="110" spans="3:29">
+      <c r="AE109" s="2"/>
+    </row>
+    <row r="110" spans="3:31">
       <c r="C110">
         <f>112/2</f>
         <v>56</v>
@@ -4566,13 +4798,13 @@
         <v>1</v>
       </c>
       <c r="N110" s="2">
-        <v>3.6819999999999999</v>
+        <v>3.6440000000000001</v>
       </c>
       <c r="O110" s="2">
-        <v>0.89900000000000002</v>
+        <v>0.90200000000000002</v>
       </c>
       <c r="P110" s="2">
-        <v>1.635</v>
+        <v>1.6439999999999999</v>
       </c>
       <c r="R110" s="4">
         <f t="shared" si="3"/>
@@ -4584,27 +4816,27 @@
       </c>
       <c r="T110" s="2">
         <f t="shared" ref="T110:T113" si="11">N110+O110+P110</f>
-        <v>6.2159999999999993</v>
+        <v>6.19</v>
       </c>
       <c r="U110" s="2">
         <f t="shared" si="5"/>
-        <v>4.0188768365019012</v>
+        <v>4.0607860900109767</v>
       </c>
       <c r="V110" s="2">
         <f t="shared" si="7"/>
-        <v>16.459960525027807</v>
+        <v>16.405215645232815</v>
       </c>
       <c r="W110" s="2">
         <f t="shared" si="6"/>
-        <v>9.0504614752293566</v>
+        <v>9.0009151532846712</v>
       </c>
       <c r="X110" s="1" t="s">
         <v>37</v>
       </c>
       <c r="AA110" s="2"/>
-      <c r="AC110" s="2"/>
-    </row>
-    <row r="111" spans="3:29">
+      <c r="AE110" s="2"/>
+    </row>
+    <row r="111" spans="3:31">
       <c r="C111">
         <f>56/2</f>
         <v>28</v>
@@ -4640,13 +4872,13 @@
         <v>1</v>
       </c>
       <c r="N111" s="2">
-        <v>0.97699999999999998</v>
+        <v>0.98499999999999999</v>
       </c>
       <c r="O111" s="2">
-        <v>0.89400000000000002</v>
+        <v>0.89700000000000002</v>
       </c>
       <c r="P111" s="2">
-        <v>1.8720000000000001</v>
+        <v>1.8819999999999999</v>
       </c>
       <c r="R111" s="4">
         <f t="shared" si="3"/>
@@ -4658,27 +4890,27 @@
       </c>
       <c r="T111" s="2">
         <f t="shared" si="11"/>
-        <v>3.7430000000000003</v>
+        <v>3.7640000000000002</v>
       </c>
       <c r="U111" s="2">
         <f t="shared" si="5"/>
-        <v>15.145859275332651</v>
+        <v>15.022847220304568</v>
       </c>
       <c r="V111" s="2">
         <f t="shared" si="7"/>
-        <v>16.552018469798657</v>
+        <v>16.496660548494983</v>
       </c>
       <c r="W111" s="2">
         <f t="shared" si="6"/>
-        <v>7.9046498461538457</v>
+        <v>7.8626485185972372</v>
       </c>
       <c r="X111" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AA111" s="2"/>
-      <c r="AC111" s="2"/>
-    </row>
-    <row r="112" spans="3:29">
+      <c r="AE111" s="2"/>
+    </row>
+    <row r="112" spans="3:31">
       <c r="C112">
         <v>14</v>
       </c>
@@ -4713,13 +4945,13 @@
         <v>1</v>
       </c>
       <c r="N112" s="2">
-        <v>0.53200000000000003</v>
+        <v>0.51800000000000002</v>
       </c>
       <c r="O112" s="2">
-        <v>0.495</v>
+        <v>0.48899999999999999</v>
       </c>
       <c r="P112" s="2">
-        <v>1.236</v>
+        <v>1.232</v>
       </c>
       <c r="R112" s="4">
         <f t="shared" si="3"/>
@@ -4731,27 +4963,27 @@
       </c>
       <c r="T112" s="2">
         <f t="shared" si="11"/>
-        <v>2.2629999999999999</v>
+        <v>2.2389999999999999</v>
       </c>
       <c r="U112" s="2">
         <f t="shared" si="5"/>
-        <v>13.907429052631578</v>
+        <v>14.283305513513513</v>
       </c>
       <c r="V112" s="2">
         <f t="shared" si="7"/>
-        <v>14.946974254545456</v>
+        <v>15.130372711656443</v>
       </c>
       <c r="W112" s="2">
         <f t="shared" si="6"/>
-        <v>5.9860455145631075</v>
+        <v>6.0054807272727277</v>
       </c>
       <c r="X112" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AA112" s="2"/>
-      <c r="AC112" s="2"/>
-    </row>
-    <row r="113" spans="3:29">
+      <c r="AE112" s="2"/>
+    </row>
+    <row r="113" spans="3:31">
       <c r="C113">
         <v>7</v>
       </c>
@@ -4786,13 +5018,13 @@
         <v>1</v>
       </c>
       <c r="N113" s="2">
-        <v>0.38</v>
+        <v>0.38100000000000001</v>
       </c>
       <c r="O113" s="2">
-        <v>0.34699999999999998</v>
+        <v>0.36799999999999999</v>
       </c>
       <c r="P113" s="2">
-        <v>0.55100000000000005</v>
+        <v>0.55300000000000005</v>
       </c>
       <c r="R113" s="4">
         <f t="shared" si="3"/>
@@ -4804,27 +5036,27 @@
       </c>
       <c r="T113" s="2">
         <f t="shared" si="11"/>
-        <v>1.278</v>
+        <v>1.302</v>
       </c>
       <c r="U113" s="2">
         <f t="shared" si="5"/>
-        <v>4.8676001684210526</v>
+        <v>4.8548243149606298</v>
       </c>
       <c r="V113" s="2">
         <f t="shared" si="7"/>
-        <v>5.3305131527377529</v>
+        <v>5.0263262608695651</v>
       </c>
       <c r="W113" s="2">
         <f t="shared" si="6"/>
-        <v>3.3569656333938291</v>
+        <v>3.3448247088607594</v>
       </c>
       <c r="X113" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AA113" s="2"/>
-      <c r="AC113" s="2"/>
-    </row>
-    <row r="114" spans="3:29">
+      <c r="AE113" s="2"/>
+    </row>
+    <row r="114" spans="3:31">
       <c r="C114">
         <v>224</v>
       </c>
@@ -4859,13 +5091,13 @@
         <v>1</v>
       </c>
       <c r="N114" s="2">
-        <v>0.77100000000000002</v>
+        <v>0.77400000000000002</v>
       </c>
       <c r="O114" s="2" t="s">
         <v>60</v>
       </c>
       <c r="P114" s="2">
-        <v>3.218</v>
+        <v>3.198</v>
       </c>
       <c r="R114" s="4">
         <f t="shared" si="3"/>
@@ -4877,26 +5109,26 @@
       </c>
       <c r="T114" s="2">
         <f>N114+P114</f>
-        <v>3.9889999999999999</v>
+        <v>3.972</v>
       </c>
       <c r="U114" s="2">
         <f t="shared" si="5"/>
-        <v>3.5986149105058365</v>
+        <v>3.5846667906976744</v>
       </c>
       <c r="V114" s="2" t="s">
         <v>60</v>
       </c>
       <c r="W114" s="2">
         <f t="shared" si="6"/>
-        <v>0.86219145307644507</v>
+        <v>0.8675835196998124</v>
       </c>
       <c r="X114" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA114" s="2"/>
-      <c r="AC114" s="2"/>
-    </row>
-    <row r="115" spans="3:29">
+      <c r="AE114" s="2"/>
+    </row>
+    <row r="115" spans="3:31">
       <c r="C115">
         <v>112</v>
       </c>
@@ -4931,13 +5163,13 @@
         <v>1</v>
       </c>
       <c r="N115" s="2">
-        <v>1.954</v>
+        <v>1.958</v>
       </c>
       <c r="O115" s="2">
-        <v>1.7849999999999999</v>
+        <v>1.7829999999999999</v>
       </c>
       <c r="P115" s="2">
-        <v>3.4420000000000002</v>
+        <v>3.4529999999999998</v>
       </c>
       <c r="R115" s="4">
         <f t="shared" si="3"/>
@@ -4949,27 +5181,27 @@
       </c>
       <c r="T115" s="2">
         <f>N115+O115+P115</f>
-        <v>7.181</v>
+        <v>7.1939999999999991</v>
       </c>
       <c r="U115" s="2">
         <f t="shared" si="5"/>
-        <v>15.145859275332651</v>
+        <v>15.114917785495402</v>
       </c>
       <c r="V115" s="2">
         <f t="shared" si="7"/>
-        <v>16.579836988235297</v>
+        <v>16.598434674144702</v>
       </c>
       <c r="W115" s="2">
         <f t="shared" si="6"/>
-        <v>8.5982013434049964</v>
+        <v>8.5708106064291929</v>
       </c>
       <c r="X115" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AA115" s="2"/>
-      <c r="AC115" s="2"/>
-    </row>
-    <row r="116" spans="3:29">
+      <c r="AE115" s="2"/>
+    </row>
+    <row r="116" spans="3:31">
       <c r="C116">
         <f>112/2</f>
         <v>56</v>
@@ -5005,13 +5237,13 @@
         <v>1</v>
       </c>
       <c r="N116" s="2">
-        <v>5.8040000000000003</v>
+        <v>5.82</v>
       </c>
       <c r="O116" s="2">
-        <v>6.0359999999999996</v>
+        <v>5.9859999999999998</v>
       </c>
       <c r="P116" s="2">
-        <v>3.1549999999999998</v>
+        <v>3.149</v>
       </c>
       <c r="R116" s="4">
         <f t="shared" si="3"/>
@@ -5023,27 +5255,27 @@
       </c>
       <c r="T116" s="2">
         <f t="shared" ref="T116:T119" si="12">N116+O116+P116</f>
-        <v>14.994999999999999</v>
+        <v>14.955000000000002</v>
       </c>
       <c r="U116" s="2">
         <f t="shared" si="5"/>
-        <v>5.0990711619572702</v>
+        <v>5.0850530969072159</v>
       </c>
       <c r="V116" s="2">
         <f t="shared" si="7"/>
-        <v>4.9030830059642145</v>
+        <v>4.9440375917139994</v>
       </c>
       <c r="W116" s="2">
         <f t="shared" si="6"/>
-        <v>9.380351513153725</v>
+        <v>9.398224523340744</v>
       </c>
       <c r="X116" s="1" t="s">
         <v>37</v>
       </c>
       <c r="AA116" s="2"/>
-      <c r="AC116" s="2"/>
-    </row>
-    <row r="117" spans="3:29">
+      <c r="AE116" s="2"/>
+    </row>
+    <row r="117" spans="3:31">
       <c r="C117">
         <f>56/2</f>
         <v>28</v>
@@ -5079,13 +5311,13 @@
         <v>1</v>
       </c>
       <c r="N117" s="2">
-        <v>2.0019999999999998</v>
+        <v>2.0169999999999999</v>
       </c>
       <c r="O117" s="2">
-        <v>1.7849999999999999</v>
+        <v>1.825</v>
       </c>
       <c r="P117" s="2">
-        <v>3.5640000000000001</v>
+        <v>3.5550000000000002</v>
       </c>
       <c r="R117" s="4">
         <f t="shared" si="3"/>
@@ -5097,27 +5329,27 @@
       </c>
       <c r="T117" s="2">
         <f t="shared" si="12"/>
-        <v>7.351</v>
+        <v>7.3970000000000002</v>
       </c>
       <c r="U117" s="2">
         <f t="shared" si="5"/>
-        <v>14.782721790209791</v>
+        <v>14.672785832424395</v>
       </c>
       <c r="V117" s="2">
         <f t="shared" si="7"/>
-        <v>16.579836988235297</v>
+        <v>16.216443300821918</v>
       </c>
       <c r="W117" s="2">
         <f t="shared" si="6"/>
-        <v>8.3038745858585852</v>
+        <v>8.3248970531645572</v>
       </c>
       <c r="X117" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AA117" s="2"/>
-      <c r="AC117" s="2"/>
-    </row>
-    <row r="118" spans="3:29">
+      <c r="AE117" s="2"/>
+    </row>
+    <row r="118" spans="3:31">
       <c r="C118">
         <v>14</v>
       </c>
@@ -5152,13 +5384,13 @@
         <v>1</v>
       </c>
       <c r="N118" s="2">
-        <v>0.97299999999999998</v>
+        <v>0.97399999999999998</v>
       </c>
       <c r="O118" s="2">
         <v>0.94899999999999995</v>
       </c>
       <c r="P118" s="2">
-        <v>1.903</v>
+        <v>1.883</v>
       </c>
       <c r="R118" s="4">
         <f t="shared" si="3"/>
@@ -5170,11 +5402,11 @@
       </c>
       <c r="T118" s="2">
         <f t="shared" si="12"/>
-        <v>3.8250000000000002</v>
+        <v>3.806</v>
       </c>
       <c r="U118" s="2">
         <f t="shared" si="5"/>
-        <v>15.208123856115108</v>
+        <v>15.192509765913758</v>
       </c>
       <c r="V118" s="2">
         <f t="shared" si="7"/>
@@ -5182,15 +5414,15 @@
       </c>
       <c r="W118" s="2">
         <f t="shared" si="6"/>
-        <v>7.7758825601681556</v>
+        <v>7.8584729219330862</v>
       </c>
       <c r="X118" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AA118" s="2"/>
-      <c r="AC118" s="2"/>
-    </row>
-    <row r="119" spans="3:29">
+      <c r="AE118" s="2"/>
+    </row>
+    <row r="119" spans="3:31">
       <c r="C119">
         <v>7</v>
       </c>
@@ -5225,13 +5457,13 @@
         <v>1</v>
       </c>
       <c r="N119" s="2">
-        <v>0.629</v>
+        <v>0.63400000000000001</v>
       </c>
       <c r="O119" s="2">
-        <v>0.57299999999999995</v>
+        <v>0.57399999999999995</v>
       </c>
       <c r="P119" s="2">
-        <v>1.724</v>
+        <v>1.7230000000000001</v>
       </c>
       <c r="R119" s="4">
         <f t="shared" si="3"/>
@@ -5243,27 +5475,27 @@
       </c>
       <c r="T119" s="2">
         <f t="shared" si="12"/>
-        <v>2.9260000000000002</v>
+        <v>2.931</v>
       </c>
       <c r="U119" s="2">
         <f t="shared" si="5"/>
-        <v>5.8813610937996819</v>
+        <v>5.8349781198738171</v>
       </c>
       <c r="V119" s="2">
         <f t="shared" si="7"/>
-        <v>6.4561538010471207</v>
+        <v>6.4449061463414639</v>
       </c>
       <c r="W119" s="2">
         <f t="shared" si="6"/>
-        <v>2.1458098190255219</v>
+        <v>2.1470552106790479</v>
       </c>
       <c r="X119" s="1" t="s">
         <v>36</v>
       </c>
       <c r="AA119" s="2"/>
-      <c r="AC119" s="2"/>
-    </row>
-    <row r="120" spans="3:29">
+      <c r="AE119" s="2"/>
+    </row>
+    <row r="120" spans="3:31">
       <c r="C120">
         <v>224</v>
       </c>
@@ -5304,7 +5536,7 @@
         <v>60</v>
       </c>
       <c r="P120" s="2">
-        <v>1.107</v>
+        <v>1.1020000000000001</v>
       </c>
       <c r="R120" s="4">
         <f t="shared" si="3"/>
@@ -5316,7 +5548,7 @@
       </c>
       <c r="T120" s="2">
         <f>N120+P120</f>
-        <v>1.605</v>
+        <v>1.6</v>
       </c>
       <c r="U120" s="2">
         <f t="shared" si="5"/>
@@ -5327,15 +5559,15 @@
       </c>
       <c r="W120" s="2">
         <f t="shared" si="6"/>
-        <v>3.4114240867208676</v>
+        <v>3.4269024174228671</v>
       </c>
       <c r="X120" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA120" s="2"/>
-      <c r="AC120" s="2"/>
-    </row>
-    <row r="121" spans="3:29">
+      <c r="AE120" s="2"/>
+    </row>
+    <row r="121" spans="3:31">
       <c r="C121">
         <v>28</v>
       </c>
@@ -5370,13 +5602,13 @@
         <v>1</v>
       </c>
       <c r="N121" s="2">
-        <v>0.58499999999999996</v>
+        <v>0.59699999999999998</v>
       </c>
       <c r="O121" s="2">
         <v>0.38900000000000001</v>
       </c>
       <c r="P121" s="2">
-        <v>0.59599999999999997</v>
+        <v>0.59399999999999997</v>
       </c>
       <c r="R121" s="4">
         <f t="shared" si="3"/>
@@ -5388,11 +5620,11 @@
       </c>
       <c r="T121" s="2">
         <f>N121+O121+P121</f>
-        <v>1.5699999999999998</v>
+        <v>1.58</v>
       </c>
       <c r="U121" s="2">
         <f t="shared" si="5"/>
-        <v>6.5872082051282055</v>
+        <v>6.4548020100502512</v>
       </c>
       <c r="V121" s="2">
         <f t="shared" si="7"/>
@@ -5400,15 +5632,15 @@
       </c>
       <c r="W121" s="2">
         <f t="shared" si="6"/>
-        <v>6.465632214765102</v>
+        <v>6.4874020202020199</v>
       </c>
       <c r="X121" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA121" s="2"/>
-      <c r="AC121" s="2"/>
-    </row>
-    <row r="122" spans="3:29">
+      <c r="AE121" s="2"/>
+    </row>
+    <row r="122" spans="3:31">
       <c r="C122">
         <v>28</v>
       </c>
@@ -5449,7 +5681,7 @@
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="P122" s="2">
-        <v>0.14899999999999999</v>
+        <v>0.14699999999999999</v>
       </c>
       <c r="R122" s="4">
         <f t="shared" si="3"/>
@@ -5461,7 +5693,7 @@
       </c>
       <c r="T122" s="2">
         <f t="shared" ref="T122:T126" si="13">N122+O122+P122</f>
-        <v>0.29000000000000004</v>
+        <v>0.28800000000000003</v>
       </c>
       <c r="U122" s="2">
         <f t="shared" si="5"/>
@@ -5473,15 +5705,15 @@
       </c>
       <c r="W122" s="2">
         <f t="shared" si="6"/>
-        <v>2.0690023087248322</v>
+        <v>2.0971519999999999</v>
       </c>
       <c r="X122" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA122" s="2"/>
-      <c r="AC122" s="2"/>
-    </row>
-    <row r="123" spans="3:29">
+      <c r="AE122" s="2"/>
+    </row>
+    <row r="123" spans="3:31">
       <c r="C123">
         <v>14</v>
       </c>
@@ -5516,13 +5748,13 @@
         <v>1</v>
       </c>
       <c r="N123" s="2">
-        <v>1.464</v>
+        <v>1.4570000000000001</v>
       </c>
       <c r="O123" s="2">
-        <v>1.2410000000000001</v>
+        <v>1.246</v>
       </c>
       <c r="P123" s="2">
-        <v>1.29</v>
+        <v>1.2529999999999999</v>
       </c>
       <c r="R123" s="4">
         <f t="shared" si="3"/>
@@ -5534,27 +5766,27 @@
       </c>
       <c r="T123" s="2">
         <f t="shared" si="13"/>
-        <v>3.9950000000000001</v>
+        <v>3.9560000000000004</v>
       </c>
       <c r="U123" s="2">
         <f t="shared" si="5"/>
-        <v>2.6321836065573772</v>
+        <v>2.6448296499656827</v>
       </c>
       <c r="V123" s="2">
         <f t="shared" si="7"/>
-        <v>3.1051706688154712</v>
+        <v>3.0927101123595508</v>
       </c>
       <c r="W123" s="2">
         <f t="shared" si="6"/>
-        <v>2.9872223255813952</v>
+        <v>3.0754324022346369</v>
       </c>
       <c r="X123" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA123" s="2"/>
-      <c r="AC123" s="2"/>
-    </row>
-    <row r="124" spans="3:29">
+      <c r="AE123" s="2"/>
+    </row>
+    <row r="124" spans="3:31">
       <c r="C124">
         <v>14</v>
       </c>
@@ -5589,13 +5821,13 @@
         <v>1</v>
       </c>
       <c r="N124" s="2">
-        <v>0.09</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="O124" s="2">
         <v>0.09</v>
       </c>
       <c r="P124" s="2">
-        <v>0.16600000000000001</v>
+        <v>0.16400000000000001</v>
       </c>
       <c r="R124" s="4">
         <f t="shared" si="3"/>
@@ -5607,11 +5839,11 @@
       </c>
       <c r="T124" s="2">
         <f t="shared" si="13"/>
-        <v>0.34599999999999997</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="U124" s="2">
         <f t="shared" si="5"/>
-        <v>6.8506965333333341</v>
+        <v>6.7754141538461532</v>
       </c>
       <c r="V124" s="2">
         <f t="shared" si="7"/>
@@ -5619,15 +5851,15 @@
       </c>
       <c r="W124" s="2">
         <f t="shared" si="6"/>
-        <v>3.7142330602409639</v>
+        <v>3.7595285853658535</v>
       </c>
       <c r="X124" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA124" s="2"/>
-      <c r="AC124" s="2"/>
-    </row>
-    <row r="125" spans="3:29">
+      <c r="AE124" s="2"/>
+    </row>
+    <row r="125" spans="3:31">
       <c r="C125">
         <v>7</v>
       </c>
@@ -5665,10 +5897,10 @@
         <v>0.10199999999999999</v>
       </c>
       <c r="O125" s="2">
-        <v>6.0999999999999999E-2</v>
+        <v>6.2E-2</v>
       </c>
       <c r="P125" s="2">
-        <v>9.8000000000000004E-2</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="R125" s="4">
         <f t="shared" si="3"/>
@@ -5680,7 +5912,7 @@
       </c>
       <c r="T125" s="2">
         <f t="shared" si="13"/>
-        <v>0.26100000000000001</v>
+        <v>0.26300000000000001</v>
       </c>
       <c r="U125" s="2">
         <f t="shared" si="5"/>
@@ -5688,19 +5920,19 @@
       </c>
       <c r="V125" s="2">
         <f t="shared" si="7"/>
-        <v>5.4749419016393448</v>
+        <v>5.3866363870967744</v>
       </c>
       <c r="W125" s="2">
         <f t="shared" si="6"/>
-        <v>3.4078719999999993</v>
+        <v>3.3734490505050503</v>
       </c>
       <c r="X125" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA125" s="2"/>
-      <c r="AC125" s="2"/>
-    </row>
-    <row r="126" spans="3:29">
+      <c r="AE125" s="2"/>
+    </row>
+    <row r="126" spans="3:31">
       <c r="C126">
         <v>7</v>
       </c>
@@ -5738,10 +5970,10 @@
         <v>0.55500000000000005</v>
       </c>
       <c r="O126" s="2">
-        <v>1.145</v>
+        <v>1.1459999999999999</v>
       </c>
       <c r="P126" s="2">
-        <v>0.78200000000000003</v>
+        <v>0.78400000000000003</v>
       </c>
       <c r="R126" s="4">
         <f t="shared" si="3"/>
@@ -5753,7 +5985,7 @@
       </c>
       <c r="T126" s="2">
         <f t="shared" si="13"/>
-        <v>2.4820000000000002</v>
+        <v>2.4850000000000003</v>
       </c>
       <c r="U126" s="2">
         <f t="shared" si="5"/>
@@ -5761,17 +5993,17 @@
       </c>
       <c r="V126" s="2">
         <f t="shared" si="7"/>
-        <v>3.6459765938864628</v>
+        <v>3.6427951134380461</v>
       </c>
       <c r="W126" s="2">
         <f t="shared" si="6"/>
-        <v>5.3384184143222502</v>
+        <v>5.3247999999999989</v>
       </c>
       <c r="X126" s="1" t="s">
         <v>35</v>
       </c>
       <c r="AA126" s="2"/>
-      <c r="AC126" s="2"/>
+      <c r="AE126" s="2"/>
     </row>
     <row r="129" spans="1:12">
       <c r="D129" t="s">
@@ -5818,18 +6050,18 @@
         <v>50</v>
       </c>
       <c r="G138" s="2">
-        <v>4.3460000000000001</v>
+        <v>4.32</v>
       </c>
       <c r="H138" s="2">
-        <v>4.1360000000000001</v>
+        <v>4.0960000000000001</v>
       </c>
       <c r="I138" s="2">
         <f>(2*$E138*$D138*$C138*$C138+$E138*$D138*$C138)/(G138/1000)/10^12</f>
-        <v>1.1407197422917625</v>
+        <v>1.147585185185185</v>
       </c>
       <c r="J138" s="2">
         <f>(2*$E138*$D138*$C138*$C138+$E138*$D138*$C138)/(H138/1000)/10^12</f>
-        <v>1.1986382978723404</v>
+        <v>1.2103437500000001</v>
       </c>
     </row>
     <row r="139" spans="1:12">
@@ -5843,18 +6075,18 @@
         <v>50</v>
       </c>
       <c r="G139" s="2">
-        <v>9.4580000000000002</v>
+        <v>8.7520000000000007</v>
       </c>
       <c r="H139" s="2">
-        <v>9.452</v>
+        <v>9.3390000000000004</v>
       </c>
       <c r="I139" s="2">
         <f t="shared" ref="I139:J149" si="14">(2*$E139*$D139*$C139*$C139+$E139*$D139*$C139)/(G139/1000)/10^12</f>
-        <v>1.0483332628462678</v>
+        <v>1.1328994515539303</v>
       </c>
       <c r="J139" s="2">
         <f t="shared" si="14"/>
-        <v>1.0489987304274226</v>
+        <v>1.0616914016489989</v>
       </c>
     </row>
     <row r="140" spans="1:12">
@@ -5897,18 +6129,18 @@
         <v>50</v>
       </c>
       <c r="G141" s="2">
-        <v>12.129</v>
+        <v>12.007999999999999</v>
       </c>
       <c r="H141" s="2">
-        <v>9.6180000000000003</v>
+        <v>10.028</v>
       </c>
       <c r="I141" s="2">
         <f t="shared" si="14"/>
-        <v>3.2698939731222691</v>
+        <v>3.3028434377081948</v>
       </c>
       <c r="J141" s="2">
         <f t="shared" si="14"/>
-        <v>4.1235749636098982</v>
+        <v>3.9549804547267646</v>
       </c>
     </row>
     <row r="142" spans="1:12">
@@ -5922,18 +6154,18 @@
         <v>50</v>
       </c>
       <c r="G142" s="2">
-        <v>6.7039999999999997</v>
+        <v>6.7720000000000002</v>
       </c>
       <c r="H142" s="2">
-        <v>6.65</v>
+        <v>6.7670000000000003</v>
       </c>
       <c r="I142" s="2">
         <f t="shared" si="14"/>
-        <v>1.001271599045346</v>
+        <v>0.99121748375664498</v>
       </c>
       <c r="J142" s="2">
         <f t="shared" si="14"/>
-        <v>1.0094022255639097</v>
+        <v>0.99194987439042404</v>
       </c>
     </row>
     <row r="143" spans="1:12">
@@ -5947,18 +6179,18 @@
         <v>50</v>
       </c>
       <c r="G143" s="2">
-        <v>9.4550000000000001</v>
+        <v>10.119</v>
       </c>
       <c r="H143" s="2">
-        <v>9.3659999999999997</v>
+        <v>9.9939999999999998</v>
       </c>
       <c r="I143" s="2">
         <f t="shared" si="14"/>
-        <v>1.4198889053410892</v>
+        <v>1.3267170273742466</v>
       </c>
       <c r="J143" s="2">
         <f t="shared" si="14"/>
-        <v>1.4333813367499468</v>
+        <v>1.3433109465679409</v>
       </c>
     </row>
     <row r="144" spans="1:12">
@@ -5972,18 +6204,18 @@
         <v>50</v>
       </c>
       <c r="G144" s="2">
-        <v>15.457000000000001</v>
+        <v>15.912000000000001</v>
       </c>
       <c r="H144" s="2">
-        <v>15.26</v>
+        <v>15.396000000000001</v>
       </c>
       <c r="I144" s="2">
         <f t="shared" si="14"/>
-        <v>1.7370834702723683</v>
+        <v>1.6874119658119655</v>
       </c>
       <c r="J144" s="2">
         <f t="shared" si="14"/>
-        <v>1.7595084665792922</v>
+        <v>1.743965913224214</v>
       </c>
     </row>
     <row r="145" spans="1:10">
@@ -6001,18 +6233,18 @@
         <v>50</v>
       </c>
       <c r="G145" s="2">
-        <v>13.981</v>
+        <v>14.18</v>
       </c>
       <c r="H145" s="2">
-        <v>10.978</v>
+        <v>11.316000000000001</v>
       </c>
       <c r="I145" s="2">
         <f t="shared" si="14"/>
-        <v>3.8409411630069381</v>
+        <v>3.787037968970381</v>
       </c>
       <c r="J145" s="2">
         <f t="shared" si="14"/>
-        <v>4.8916194570960094</v>
+        <v>4.7455106398020499</v>
       </c>
     </row>
     <row r="146" spans="1:10">
@@ -6026,18 +6258,18 @@
         <v>50</v>
       </c>
       <c r="G146" s="2">
-        <v>10.565</v>
+        <v>10.563000000000001</v>
       </c>
       <c r="H146" s="2">
-        <v>10.372999999999999</v>
+        <v>10.288</v>
       </c>
       <c r="I146" s="2">
         <f t="shared" si="14"/>
-        <v>0.99269361097964981</v>
+        <v>0.99288156773643832</v>
       </c>
       <c r="J146" s="2">
         <f t="shared" si="14"/>
-        <v>1.0110679649088983</v>
+        <v>1.0194214618973561</v>
       </c>
     </row>
     <row r="147" spans="1:10">
@@ -6051,18 +6283,18 @@
         <v>50</v>
       </c>
       <c r="G147" s="2">
-        <v>12.382</v>
+        <v>12.906000000000001</v>
       </c>
       <c r="H147" s="2">
-        <v>12.308999999999999</v>
+        <v>12.74</v>
       </c>
       <c r="I147" s="2">
         <f t="shared" si="14"/>
-        <v>1.6940410272976905</v>
+        <v>1.6252608089260807</v>
       </c>
       <c r="J147" s="2">
         <f t="shared" si="14"/>
-        <v>1.7040877406775532</v>
+        <v>1.6464376766091051</v>
       </c>
     </row>
     <row r="148" spans="1:10">
@@ -6076,18 +6308,18 @@
         <v>50</v>
       </c>
       <c r="G148" s="2">
-        <v>18.138999999999999</v>
+        <v>18.486999999999998</v>
       </c>
       <c r="H148" s="2">
-        <v>17.843</v>
+        <v>18.085000000000001</v>
       </c>
       <c r="I148" s="2">
         <f t="shared" si="14"/>
-        <v>2.3127643199735375</v>
+        <v>2.2692287553415915</v>
       </c>
       <c r="J148" s="2">
         <f t="shared" si="14"/>
-        <v>2.3511310878215546</v>
+        <v>2.3196700027647221</v>
       </c>
     </row>
     <row r="149" spans="1:10">
@@ -6101,18 +6333,18 @@
         <v>50</v>
       </c>
       <c r="G149" s="2">
-        <v>17.562999999999999</v>
+        <v>16.983000000000001</v>
       </c>
       <c r="H149" s="2">
-        <v>13.837</v>
+        <v>14.29</v>
       </c>
       <c r="I149" s="2">
         <f t="shared" si="14"/>
-        <v>4.7772284917155394</v>
+        <v>4.9403794382617914</v>
       </c>
       <c r="J149" s="2">
         <f t="shared" si="14"/>
-        <v>6.0636311339163118</v>
+        <v>5.8714110566829953</v>
       </c>
     </row>
     <row r="153" spans="1:10">
@@ -6152,18 +6384,18 @@
         <v>25</v>
       </c>
       <c r="G154" s="2">
-        <v>1.508</v>
+        <v>1.5589999999999999</v>
       </c>
       <c r="H154" s="2">
-        <v>1.9770000000000001</v>
+        <v>1.9359999999999999</v>
       </c>
       <c r="I154" s="2">
-        <f>(8*$E154*$D154*$C154*$C154)/(G154/1000)/10^12</f>
-        <v>0.55627374005305041</v>
+        <f t="shared" ref="I154:I169" si="15">(8*$E154*$D154*$C154*$C154)/(G154/1000)/10^12</f>
+        <v>0.53807620269403467</v>
       </c>
       <c r="J154" s="2">
-        <f>(8*$E154*$D154*$C154*$C154)/(H154/1000)/10^12</f>
-        <v>0.42430996459281739</v>
+        <f t="shared" ref="J154:J169" si="16">(8*$E154*$D154*$C154*$C154)/(H154/1000)/10^12</f>
+        <v>0.43329586776859502</v>
       </c>
     </row>
     <row r="155" spans="1:10">
@@ -6177,18 +6409,18 @@
         <v>25</v>
       </c>
       <c r="G155" s="2">
-        <v>2.82</v>
+        <v>2.7610000000000001</v>
       </c>
       <c r="H155" s="2">
-        <v>4.0140000000000002</v>
+        <v>3.9689999999999999</v>
       </c>
       <c r="I155" s="2">
-        <f t="shared" ref="I155:I169" si="15">(8*$E155*$D155*$C155*$C155)/(G155/1000)/10^12</f>
-        <v>0.59493673758865251</v>
+        <f t="shared" si="15"/>
+        <v>0.60764998189061936</v>
       </c>
       <c r="J155" s="2">
-        <f t="shared" ref="J155:J169" si="16">(8*$E155*$D155*$C155*$C155)/(H155/1000)/10^12</f>
-        <v>0.41796751370204283</v>
+        <f t="shared" si="16"/>
+        <v>0.42270637440161257</v>
       </c>
     </row>
     <row r="156" spans="1:10">
@@ -6202,18 +6434,18 @@
         <v>25</v>
       </c>
       <c r="G156" s="2">
-        <v>2.2930000000000001</v>
+        <v>2.347</v>
       </c>
       <c r="H156" s="2">
-        <v>4.024</v>
+        <v>3.992</v>
       </c>
       <c r="I156" s="2">
         <f t="shared" si="15"/>
-        <v>1.4633419973833404</v>
+        <v>1.4296732850447378</v>
       </c>
       <c r="J156" s="2">
         <f t="shared" si="16"/>
-        <v>0.83385765407554679</v>
+        <v>0.84054188376753503</v>
       </c>
     </row>
     <row r="157" spans="1:10">
@@ -6227,18 +6459,18 @@
         <v>25</v>
       </c>
       <c r="G157" s="2">
-        <v>2.4289999999999998</v>
+        <v>2.67</v>
       </c>
       <c r="H157" s="2">
-        <v>4.93</v>
+        <v>4.9889999999999999</v>
       </c>
       <c r="I157" s="2">
         <f t="shared" si="15"/>
-        <v>2.7628186084808566</v>
+        <v>2.5134405992509361</v>
       </c>
       <c r="J157" s="2">
         <f t="shared" si="16"/>
-        <v>1.3612345638945234</v>
+        <v>1.3451365804770496</v>
       </c>
     </row>
     <row r="158" spans="1:10">
@@ -6252,18 +6484,18 @@
         <v>25</v>
       </c>
       <c r="G158" s="2">
-        <v>4.6230000000000002</v>
+        <v>4.6369999999999996</v>
       </c>
       <c r="H158" s="2">
-        <v>2.8250000000000002</v>
+        <v>2.855</v>
       </c>
       <c r="I158" s="2">
         <f t="shared" si="15"/>
-        <v>0.72581509842093872</v>
+        <v>0.72362372223420324</v>
       </c>
       <c r="J158" s="2">
         <f t="shared" si="16"/>
-        <v>1.1877675044247786</v>
+        <v>1.1752865849387042</v>
       </c>
     </row>
     <row r="159" spans="1:10">
@@ -6277,18 +6509,18 @@
         <v>25</v>
       </c>
       <c r="G159" s="2">
-        <v>4.5419999999999998</v>
+        <v>4.5620000000000003</v>
       </c>
       <c r="H159" s="2">
-        <v>5.22</v>
+        <v>5.173</v>
       </c>
       <c r="I159" s="2">
         <f t="shared" si="15"/>
-        <v>1.4775179216204315</v>
+        <v>1.4710404208680403</v>
       </c>
       <c r="J159" s="2">
         <f t="shared" si="16"/>
-        <v>1.2856104214559387</v>
+        <v>1.2972910110187512</v>
       </c>
     </row>
     <row r="160" spans="1:10">
@@ -6302,18 +6534,18 @@
         <v>25</v>
       </c>
       <c r="G160" s="2">
-        <v>4.3920000000000003</v>
+        <v>4.359</v>
       </c>
       <c r="H160" s="2">
-        <v>8.3369999999999997</v>
+        <v>8.1389999999999993</v>
       </c>
       <c r="I160" s="2">
         <f t="shared" si="15"/>
-        <v>3.055959198542805</v>
+        <v>3.0790944712089927</v>
       </c>
       <c r="J160" s="2">
         <f t="shared" si="16"/>
-        <v>1.6099043780736477</v>
+        <v>1.6490690256788305</v>
       </c>
     </row>
     <row r="161" spans="3:10">
@@ -6327,18 +6559,18 @@
         <v>25</v>
       </c>
       <c r="G161" s="2">
-        <v>4.9640000000000004</v>
+        <v>5.1719999999999997</v>
       </c>
       <c r="H161" s="2">
-        <v>11.939</v>
+        <v>11.946999999999999</v>
       </c>
       <c r="I161" s="2">
         <f t="shared" si="15"/>
-        <v>5.4076441579371464</v>
+        <v>5.1901673627223515</v>
       </c>
       <c r="J161" s="2">
         <f t="shared" si="16"/>
-        <v>2.2483914565709018</v>
+        <v>2.2468858793002426</v>
       </c>
     </row>
     <row r="162" spans="3:10">
@@ -6352,18 +6584,18 @@
         <v>25</v>
       </c>
       <c r="G162" s="2">
-        <v>20.670999999999999</v>
+        <v>20.658000000000001</v>
       </c>
       <c r="H162" s="2">
-        <v>9.8320000000000007</v>
+        <v>9.8409999999999993</v>
       </c>
       <c r="I162" s="2">
         <f t="shared" si="15"/>
-        <v>0.64930447486817289</v>
+        <v>0.64971307967857483</v>
       </c>
       <c r="J162" s="2">
         <f t="shared" si="16"/>
-        <v>1.3651111472742066</v>
+        <v>1.3638626968803984</v>
       </c>
     </row>
     <row r="163" spans="3:10">
@@ -6377,18 +6609,18 @@
         <v>25</v>
       </c>
       <c r="G163" s="2">
-        <v>13.145</v>
+        <v>13.087999999999999</v>
       </c>
       <c r="H163" s="2">
-        <v>12.04</v>
+        <v>11.788</v>
       </c>
       <c r="I163" s="2">
         <f t="shared" si="15"/>
-        <v>2.0421107341194369</v>
+        <v>2.0510044009779955</v>
       </c>
       <c r="J163" s="2">
         <f t="shared" si="16"/>
-        <v>2.2295303654485052</v>
+        <v>2.2771925347811335</v>
       </c>
     </row>
     <row r="164" spans="3:10">
@@ -6402,18 +6634,18 @@
         <v>25</v>
       </c>
       <c r="G164" s="2">
-        <v>10.09</v>
+        <v>10.186999999999999</v>
       </c>
       <c r="H164" s="2">
-        <v>19.231999999999999</v>
+        <v>19.222999999999999</v>
       </c>
       <c r="I164" s="2">
         <f t="shared" si="15"/>
-        <v>5.3208217244796829</v>
+        <v>5.2701571807205267</v>
       </c>
       <c r="J164" s="2">
         <f t="shared" si="16"/>
-        <v>2.7915500831946756</v>
+        <v>2.7928570566508868</v>
       </c>
     </row>
     <row r="165" spans="3:10">
@@ -6427,18 +6659,18 @@
         <v>25</v>
       </c>
       <c r="G165" s="2">
-        <v>16.12</v>
+        <v>16.128</v>
       </c>
       <c r="H165" s="2">
-        <v>20.81</v>
+        <v>19.62</v>
       </c>
       <c r="I165" s="2">
         <f t="shared" si="15"/>
-        <v>6.6609294292803964</v>
+        <v>6.6576253968253969</v>
       </c>
       <c r="J165" s="2">
         <f t="shared" si="16"/>
-        <v>5.1597396636232586</v>
+        <v>5.472690234454638</v>
       </c>
     </row>
     <row r="166" spans="3:10">
@@ -6452,18 +6684,18 @@
         <v>25</v>
       </c>
       <c r="G166" s="2">
-        <v>80.930999999999997</v>
+        <v>80.944999999999993</v>
       </c>
       <c r="H166" s="2">
-        <v>57.363999999999997</v>
+        <v>57.247999999999998</v>
       </c>
       <c r="I166" s="2">
         <f t="shared" si="15"/>
-        <v>0.66336868690612993</v>
+        <v>0.66325395268392129</v>
       </c>
       <c r="J166" s="2">
         <f t="shared" si="16"/>
-        <v>0.93590215466146021</v>
+        <v>0.93779854667411966</v>
       </c>
     </row>
     <row r="167" spans="3:10">
@@ -6477,18 +6709,18 @@
         <v>25</v>
       </c>
       <c r="G167" s="2">
-        <v>39.793999999999997</v>
+        <v>39.863</v>
       </c>
       <c r="H167" s="2">
-        <v>36.348999999999997</v>
+        <v>36.305</v>
       </c>
       <c r="I167" s="2">
         <f t="shared" si="15"/>
-        <v>2.6982505503342216</v>
+        <v>2.6935800717457292</v>
       </c>
       <c r="J167" s="2">
         <f t="shared" si="16"/>
-        <v>2.9539789925444988</v>
+        <v>2.957559080016527</v>
       </c>
     </row>
     <row r="168" spans="3:10">
@@ -6502,18 +6734,18 @@
         <v>25</v>
       </c>
       <c r="G168" s="2">
-        <v>32.290999999999997</v>
+        <v>32.213999999999999</v>
       </c>
       <c r="H168" s="2">
-        <v>46.613</v>
+        <v>46.113</v>
       </c>
       <c r="I168" s="2">
         <f t="shared" si="15"/>
-        <v>6.6504092409649749</v>
+        <v>6.666305482088533</v>
       </c>
       <c r="J168" s="2">
         <f t="shared" si="16"/>
-        <v>4.6070487803831544</v>
+        <v>4.6570026847093011</v>
       </c>
     </row>
     <row r="169" spans="3:10">
@@ -6527,18 +6759,18 @@
         <v>25</v>
       </c>
       <c r="G169" s="2">
-        <v>54.985999999999997</v>
+        <v>54.881999999999998</v>
       </c>
       <c r="H169" s="2">
-        <v>59.868000000000002</v>
+        <v>59.124000000000002</v>
       </c>
       <c r="I169" s="2">
         <f t="shared" si="15"/>
-        <v>7.8110197068344664</v>
+        <v>7.825821391348712</v>
       </c>
       <c r="J169" s="2">
         <f t="shared" si="16"/>
-        <v>7.1740617625442633</v>
+        <v>7.2643381638590077</v>
       </c>
     </row>
     <row r="172" spans="3:10">
@@ -6561,7 +6793,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6622,7 +6854,7 @@
         <v>52</v>
       </c>
       <c r="B7" s="9">
-        <v>367.35</v>
+        <v>367.48</v>
       </c>
     </row>
     <row r="8" spans="1:2">

</xml_diff>

<commit_message>
Fix typo in TitanX Pascal spec sheet
</commit_message>
<xml_diff>
--- a/results/DeepBench_NV_TitanX_Pascal.xlsx
+++ b/results/DeepBench_NV_TitanX_Pascal.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="14940" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="3" r:id="rId1"/>
@@ -157,9 +157,6 @@
     <t>GPU Model</t>
   </si>
   <si>
-    <t>Nvidia Tesla M40</t>
-  </si>
-  <si>
     <t>Linux Kernel Version</t>
   </si>
   <si>
@@ -209,6 +206,9 @@
   </si>
   <si>
     <t>Total Time (msec)</t>
+  </si>
+  <si>
+    <t>Nvidia TitanX Pascal</t>
   </si>
 </sst>
 </file>
@@ -1201,7 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE172"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -3367,7 +3367,7 @@
         <v>33</v>
       </c>
       <c r="T90" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U90" t="s">
         <v>38</v>
@@ -3420,7 +3420,7 @@
         <v>0.13200000000000001</v>
       </c>
       <c r="O91" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P91" s="2">
         <v>0.28000000000000003</v>
@@ -3442,7 +3442,7 @@
         <v>5.1838545454545448</v>
       </c>
       <c r="V91" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W91" s="2">
         <f>(2*$R91*$S91*$F91*$G91*$E91*$H91*$I91)/(P91/1000)/10^12</f>
@@ -3492,7 +3492,7 @@
         <v>0.23100000000000001</v>
       </c>
       <c r="O92" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P92" s="2">
         <v>0.51500000000000001</v>
@@ -3514,7 +3514,7 @@
         <v>5.9244051948051943</v>
       </c>
       <c r="V92" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W92" s="2">
         <f t="shared" ref="W92:W126" si="6">(2*$R92*$S92*$F92*$G92*$E92*$H92*$I92)/(P92/1000)/10^12</f>
@@ -3564,7 +3564,7 @@
         <v>0.41</v>
       </c>
       <c r="O93" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P93" s="2">
         <v>0.98699999999999999</v>
@@ -3586,7 +3586,7 @@
         <v>6.6757931707317066</v>
       </c>
       <c r="V93" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W93" s="2">
         <f t="shared" si="6"/>
@@ -3636,7 +3636,7 @@
         <v>0.82499999999999996</v>
       </c>
       <c r="O94" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P94" s="2">
         <v>2.1349999999999998</v>
@@ -3658,7 +3658,7 @@
         <v>6.6353338181818184</v>
       </c>
       <c r="V94" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W94" s="2">
         <f t="shared" si="6"/>
@@ -4000,7 +4000,7 @@
         <v>0.11899999999999999</v>
       </c>
       <c r="O99" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P99" s="2">
         <v>0.40600000000000003</v>
@@ -4022,7 +4022,7 @@
         <v>0.89217075630252107</v>
       </c>
       <c r="V99" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W99" s="2">
         <f t="shared" si="6"/>
@@ -4291,7 +4291,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="O103" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P103" s="2">
         <v>0.10199999999999999</v>
@@ -4313,7 +4313,7 @@
         <v>2.1789612972972972</v>
       </c>
       <c r="V103" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W103" s="2">
         <f t="shared" si="6"/>
@@ -4655,7 +4655,7 @@
         <v>0.39800000000000002</v>
       </c>
       <c r="O108" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P108" s="2">
         <v>1.611</v>
@@ -4677,7 +4677,7 @@
         <v>3.4855930854271353</v>
       </c>
       <c r="V108" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W108" s="2">
         <f t="shared" si="6"/>
@@ -5094,7 +5094,7 @@
         <v>0.77400000000000002</v>
       </c>
       <c r="O114" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P114" s="2">
         <v>3.198</v>
@@ -5116,7 +5116,7 @@
         <v>3.5846667906976744</v>
       </c>
       <c r="V114" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W114" s="2">
         <f t="shared" si="6"/>
@@ -5533,7 +5533,7 @@
         <v>0.498</v>
       </c>
       <c r="O120" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P120" s="2">
         <v>1.1020000000000001</v>
@@ -5555,7 +5555,7 @@
         <v>7.5832258313253016</v>
       </c>
       <c r="V120" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W120" s="2">
         <f t="shared" si="6"/>
@@ -6007,7 +6007,7 @@
     </row>
     <row r="129" spans="1:12">
       <c r="D129" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="135" spans="1:12">
@@ -6792,8 +6792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6806,7 +6806,7 @@
         <v>43</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6814,20 +6814,20 @@
         <v>44</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>46</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="8">
         <v>8</v>
@@ -6835,7 +6835,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="8">
         <v>5</v>
@@ -6843,15 +6843,15 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="9">
         <v>367.48</v>
@@ -6859,26 +6859,26 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
         <v>55</v>
-      </c>
-      <c r="B9" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
         <v>57</v>
-      </c>
-      <c r="B10" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>